<commit_message>
modified the submission template
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_submission_v3_13_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_submission_v3_13_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20C4D36-9047-FF4C-9712-D806B4F2CC8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779A9B7D-E1A8-1345-B983-D9AF528AA3B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleSubmission" sheetId="1" r:id="rId1"/>
@@ -65,22 +65,29 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Instructions</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Instructions
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">SampleName must be </t>
         </r>
@@ -89,9 +96,8 @@
             <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t>unique.</t>
         </r>
@@ -99,9 +105,8 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve"> If sample name is not unique, a unique prefix will be added to it. Only use the following characters for Sample name:</t>
         </r>
@@ -110,9 +115,8 @@
             <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve"> a-z, A-Z, 0-9, period (.), dash (-), underscore ( _ )</t>
         </r>
@@ -120,11 +124,19 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">. 
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -132,9 +144,8 @@
             <i/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t>Do not use any special characters</t>
         </r>
@@ -144,11 +155,10 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
+            <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Instructions:
 </t>
@@ -157,9 +167,8 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Container Name must be </t>
         </r>
@@ -168,9 +177,8 @@
             <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t>unique.</t>
         </r>
@@ -178,9 +186,8 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve"> If container name is not unique, a unique prefix will be added to it. Only use the following characters for Sample name:</t>
         </r>
@@ -189,9 +196,8 @@
             <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve"> a-z, A-Z, 0-9, period (.), dash (-), underscore ( _ )</t>
         </r>
@@ -199,11 +205,29 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">DON'T USE ANY SPECIAL </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>. DON'T USE ANY SPECIAL CHARACTERS!!</t>
+          <t>CHARACTERS!!</t>
         </r>
       </text>
     </comment>
@@ -214,8 +238,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Use the ID# only:
 </t>
@@ -224,16 +247,10 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Homo Sapiens #9606 
-Mus Musculus #10090 
-Sars-Cov-2 #2697049
-Ixodes Scapularis #6945
-Canis Lupus Familiaris #9615
-Escherichia Coli #562
 </t>
         </r>
         <r>
@@ -241,29 +258,180 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <family val="34"/>
           </rPr>
-          <t xml:space="preserve">Leishmania donovani #5661
-Borreliella burgdorferi #139
-Influenza A virus #11320 
-Influenza B virus #11520
-Respiratory syncytial virus #12814
-Pedicularis canadensis #1325716
-Passiflora #3684
-Salvelinus fontinalis #8038
-Salvelinus namaycush #8040
+          <t xml:space="preserve">Mus Musculus #10090 
 </t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
-          <t>Phaseolus vulgaris #3885</t>
+          <t xml:space="preserve">Sars-Cov-2 #2697049
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Ixodes Scapularis #6945
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Canis Lupus Familiaris #9615
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Escherichia Coli #562
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Leishmania donovani #5661
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Borreliella burgdorferi #139
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Influenza A virus #11320 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Influenza B virus #11520
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Respiratory syncytial virus #12814
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Pedicularis canadensis #1325716
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Passiflora #3684
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Salvelinus fontinalis #8038
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Salvelinus namaycush #8040
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Phaseolus vulgaris #3885
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Gasterosteus aculeatus #69293
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Gasterosteus aculeatus aculeatus #481459
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -274,8 +442,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Note: </t>
         </r>
@@ -283,9 +450,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Mandatory if sample is Nucleid Acid
 </t>
@@ -299,10 +465,38 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Note: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Mandatory if sample is Nucleic Acid. If unknown please select </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Tissue </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">category.
+</t>
         </r>
         <r>
           <rPr>
@@ -312,28 +506,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Mandatory if sample is Nucleic Acid. If unknown please select </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Tissue </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">category.
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -355,8 +528,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Instructions:
 </t>
@@ -365,9 +537,8 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Container Name must be </t>
         </r>
@@ -376,9 +547,8 @@
             <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t>unique.</t>
         </r>
@@ -386,9 +556,8 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve"> If container name is not unique, a unique prefix will be added to it. Only use the following characters for Sample name:</t>
         </r>
@@ -397,9 +566,8 @@
             <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve"> a-z, A-Z, 0-9, period (.), dash (-), underscore ( _ )</t>
         </r>
@@ -407,9 +575,8 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t>. DON'T USE ANY SPECIAL CHARACTERS!!</t>
         </r>
@@ -9202,7 +9369,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]\-0"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -9263,44 +9430,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -9340,6 +9469,57 @@
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="34"/>
     </font>
   </fonts>
   <fills count="13">
@@ -9516,28 +9696,28 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9764,8 +9944,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Taxons" displayName="Taxons" ref="G1:G17" totalsRowShown="0">
-  <autoFilter ref="G1:G17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Taxons" displayName="Taxons" ref="G1:G19" totalsRowShown="0">
+  <autoFilter ref="G1:G19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Taxon"/>
   </tableColumns>
@@ -10072,8 +10252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG500"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15"/>
@@ -27183,7 +27363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D7C4E7-7AC8-0C49-AC2B-A7A7FD552174}">
   <dimension ref="A1:J500"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -32835,7 +33015,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC385"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:G19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15"/>
   <cols>
@@ -34120,6 +34302,9 @@
       <c r="F18" t="s">
         <v>84</v>
       </c>
+      <c r="G18">
+        <v>69293</v>
+      </c>
       <c r="O18" t="s">
         <v>370</v>
       </c>
@@ -34175,6 +34360,9 @@
       </c>
       <c r="F19" t="s">
         <v>189</v>
+      </c>
+      <c r="G19">
+        <v>481459</v>
       </c>
       <c r="O19" t="s">
         <v>387</v>

</xml_diff>

<commit_message>
Added platform validation and fixed template issues
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_submission_v3_13_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_submission_v3_13_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD65E515-8837-8045-920D-DBEDD5BEFB1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55475CA-CCB5-6D4C-9E16-65E9E3E714A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9547,7 +9547,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9615,6 +9615,14 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10151,8 +10159,8 @@
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="15.5" customWidth="1"/>
     <col min="11" max="12" width="19.5" customWidth="1"/>
     <col min="13" max="14" width="15.5" customWidth="1"/>
@@ -10167,7 +10175,8 @@
     <col min="23" max="23" width="30.5" customWidth="1"/>
     <col min="24" max="24" width="19.5" customWidth="1"/>
     <col min="25" max="25" width="24.5" customWidth="1"/>
-    <col min="26" max="27" width="24" customWidth="1"/>
+    <col min="26" max="26" width="24" customWidth="1"/>
+    <col min="27" max="27" width="24" style="31" customWidth="1"/>
     <col min="28" max="28" width="41.1640625" customWidth="1"/>
     <col min="29" max="30" width="36.83203125" customWidth="1"/>
     <col min="31" max="31" width="27.6640625" customWidth="1"/>
@@ -10224,6 +10233,7 @@
       <c r="V6" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="AA6" s="32"/>
       <c r="AE6" s="5" t="s">
         <v>4</v>
       </c>
@@ -10307,7 +10317,7 @@
       <c r="Z7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AA7" s="11" t="s">
+      <c r="AA7" s="33" t="s">
         <v>2908</v>
       </c>
       <c r="AB7" s="11" t="s">
@@ -10353,7 +10363,7 @@
       <c r="X8" s="13"/>
       <c r="Y8" s="13"/>
       <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
+      <c r="AA8" s="34"/>
       <c r="AB8" s="13"/>
       <c r="AC8" s="13"/>
       <c r="AD8" s="13"/>
@@ -10387,7 +10397,7 @@
       <c r="X9" s="13"/>
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
+      <c r="AA9" s="34"/>
       <c r="AB9" s="13"/>
       <c r="AC9" s="13"/>
       <c r="AD9" s="13"/>
@@ -10421,7 +10431,7 @@
       <c r="X10" s="13"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
+      <c r="AA10" s="34"/>
       <c r="AB10" s="13"/>
       <c r="AC10" s="13"/>
       <c r="AD10" s="13"/>
@@ -10455,7 +10465,7 @@
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
       <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
+      <c r="AA11" s="34"/>
       <c r="AB11" s="13"/>
       <c r="AC11" s="13"/>
       <c r="AD11" s="13"/>
@@ -10489,7 +10499,7 @@
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
       <c r="Z12" s="13"/>
-      <c r="AA12" s="13"/>
+      <c r="AA12" s="34"/>
       <c r="AB12" s="13"/>
       <c r="AC12" s="13"/>
       <c r="AD12" s="13"/>
@@ -10523,7 +10533,7 @@
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
       <c r="Z13" s="13"/>
-      <c r="AA13" s="13"/>
+      <c r="AA13" s="34"/>
       <c r="AB13" s="13"/>
       <c r="AC13" s="13"/>
       <c r="AD13" s="13"/>
@@ -10557,7 +10567,7 @@
       <c r="X14" s="13"/>
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
-      <c r="AA14" s="13"/>
+      <c r="AA14" s="34"/>
       <c r="AB14" s="13"/>
       <c r="AC14" s="13"/>
       <c r="AD14" s="13"/>
@@ -10591,7 +10601,7 @@
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
       <c r="Z15" s="13"/>
-      <c r="AA15" s="13"/>
+      <c r="AA15" s="34"/>
       <c r="AB15" s="13"/>
       <c r="AC15" s="13"/>
       <c r="AD15" s="13"/>
@@ -10625,7 +10635,7 @@
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
-      <c r="AA16" s="13"/>
+      <c r="AA16" s="34"/>
       <c r="AB16" s="13"/>
       <c r="AC16" s="13"/>
       <c r="AD16" s="13"/>
@@ -10659,7 +10669,7 @@
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
       <c r="Z17" s="13"/>
-      <c r="AA17" s="13"/>
+      <c r="AA17" s="34"/>
       <c r="AB17" s="13"/>
       <c r="AC17" s="13"/>
       <c r="AD17" s="13"/>
@@ -10693,7 +10703,7 @@
       <c r="X18" s="13"/>
       <c r="Y18" s="13"/>
       <c r="Z18" s="13"/>
-      <c r="AA18" s="13"/>
+      <c r="AA18" s="34"/>
       <c r="AB18" s="13"/>
       <c r="AC18" s="13"/>
       <c r="AD18" s="13"/>
@@ -10727,7 +10737,7 @@
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
       <c r="Z19" s="13"/>
-      <c r="AA19" s="13"/>
+      <c r="AA19" s="34"/>
       <c r="AB19" s="13"/>
       <c r="AC19" s="13"/>
       <c r="AD19" s="13"/>
@@ -10761,7 +10771,7 @@
       <c r="X20" s="13"/>
       <c r="Y20" s="13"/>
       <c r="Z20" s="13"/>
-      <c r="AA20" s="13"/>
+      <c r="AA20" s="34"/>
       <c r="AB20" s="13"/>
       <c r="AC20" s="13"/>
       <c r="AD20" s="13"/>
@@ -10795,7 +10805,7 @@
       <c r="X21" s="13"/>
       <c r="Y21" s="13"/>
       <c r="Z21" s="13"/>
-      <c r="AA21" s="13"/>
+      <c r="AA21" s="34"/>
       <c r="AB21" s="13"/>
       <c r="AC21" s="13"/>
       <c r="AD21" s="13"/>
@@ -10829,7 +10839,7 @@
       <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
       <c r="Z22" s="13"/>
-      <c r="AA22" s="13"/>
+      <c r="AA22" s="34"/>
       <c r="AB22" s="13"/>
       <c r="AC22" s="13"/>
       <c r="AD22" s="13"/>
@@ -10863,7 +10873,7 @@
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
       <c r="Z23" s="13"/>
-      <c r="AA23" s="13"/>
+      <c r="AA23" s="34"/>
       <c r="AB23" s="13"/>
       <c r="AC23" s="13"/>
       <c r="AD23" s="13"/>
@@ -10897,7 +10907,7 @@
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
       <c r="Z24" s="13"/>
-      <c r="AA24" s="13"/>
+      <c r="AA24" s="34"/>
       <c r="AB24" s="13"/>
       <c r="AC24" s="13"/>
       <c r="AD24" s="13"/>
@@ -10931,7 +10941,7 @@
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
       <c r="Z25" s="13"/>
-      <c r="AA25" s="13"/>
+      <c r="AA25" s="34"/>
       <c r="AB25" s="13"/>
       <c r="AC25" s="13"/>
       <c r="AD25" s="13"/>
@@ -10965,7 +10975,7 @@
       <c r="X26" s="13"/>
       <c r="Y26" s="13"/>
       <c r="Z26" s="13"/>
-      <c r="AA26" s="13"/>
+      <c r="AA26" s="34"/>
       <c r="AB26" s="13"/>
       <c r="AC26" s="13"/>
       <c r="AD26" s="13"/>
@@ -10999,7 +11009,7 @@
       <c r="X27" s="13"/>
       <c r="Y27" s="13"/>
       <c r="Z27" s="13"/>
-      <c r="AA27" s="13"/>
+      <c r="AA27" s="34"/>
       <c r="AB27" s="13"/>
       <c r="AC27" s="13"/>
       <c r="AD27" s="13"/>
@@ -11033,7 +11043,7 @@
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
       <c r="Z28" s="13"/>
-      <c r="AA28" s="13"/>
+      <c r="AA28" s="34"/>
       <c r="AB28" s="13"/>
       <c r="AC28" s="13"/>
       <c r="AD28" s="13"/>
@@ -11067,7 +11077,7 @@
       <c r="X29" s="13"/>
       <c r="Y29" s="13"/>
       <c r="Z29" s="13"/>
-      <c r="AA29" s="13"/>
+      <c r="AA29" s="34"/>
       <c r="AB29" s="13"/>
       <c r="AC29" s="13"/>
       <c r="AD29" s="13"/>
@@ -11101,7 +11111,7 @@
       <c r="X30" s="13"/>
       <c r="Y30" s="13"/>
       <c r="Z30" s="13"/>
-      <c r="AA30" s="13"/>
+      <c r="AA30" s="34"/>
       <c r="AB30" s="13"/>
       <c r="AC30" s="13"/>
       <c r="AD30" s="13"/>
@@ -11135,7 +11145,7 @@
       <c r="X31" s="13"/>
       <c r="Y31" s="13"/>
       <c r="Z31" s="13"/>
-      <c r="AA31" s="13"/>
+      <c r="AA31" s="34"/>
       <c r="AB31" s="13"/>
       <c r="AC31" s="13"/>
       <c r="AD31" s="13"/>
@@ -11169,7 +11179,7 @@
       <c r="X32" s="13"/>
       <c r="Y32" s="13"/>
       <c r="Z32" s="13"/>
-      <c r="AA32" s="13"/>
+      <c r="AA32" s="34"/>
       <c r="AB32" s="13"/>
       <c r="AC32" s="13"/>
       <c r="AD32" s="13"/>
@@ -11203,7 +11213,7 @@
       <c r="X33" s="13"/>
       <c r="Y33" s="13"/>
       <c r="Z33" s="13"/>
-      <c r="AA33" s="13"/>
+      <c r="AA33" s="34"/>
       <c r="AB33" s="13"/>
       <c r="AC33" s="13"/>
       <c r="AD33" s="13"/>
@@ -11237,7 +11247,7 @@
       <c r="X34" s="13"/>
       <c r="Y34" s="13"/>
       <c r="Z34" s="13"/>
-      <c r="AA34" s="13"/>
+      <c r="AA34" s="34"/>
       <c r="AB34" s="13"/>
       <c r="AC34" s="13"/>
       <c r="AD34" s="13"/>
@@ -11271,7 +11281,7 @@
       <c r="X35" s="13"/>
       <c r="Y35" s="13"/>
       <c r="Z35" s="13"/>
-      <c r="AA35" s="13"/>
+      <c r="AA35" s="34"/>
       <c r="AB35" s="13"/>
       <c r="AC35" s="13"/>
       <c r="AD35" s="13"/>
@@ -11305,7 +11315,7 @@
       <c r="X36" s="13"/>
       <c r="Y36" s="13"/>
       <c r="Z36" s="13"/>
-      <c r="AA36" s="13"/>
+      <c r="AA36" s="34"/>
       <c r="AB36" s="13"/>
       <c r="AC36" s="13"/>
       <c r="AD36" s="13"/>
@@ -11339,7 +11349,7 @@
       <c r="X37" s="13"/>
       <c r="Y37" s="13"/>
       <c r="Z37" s="13"/>
-      <c r="AA37" s="13"/>
+      <c r="AA37" s="34"/>
       <c r="AB37" s="13"/>
       <c r="AC37" s="13"/>
       <c r="AD37" s="13"/>
@@ -11373,7 +11383,7 @@
       <c r="X38" s="13"/>
       <c r="Y38" s="13"/>
       <c r="Z38" s="13"/>
-      <c r="AA38" s="13"/>
+      <c r="AA38" s="34"/>
       <c r="AB38" s="13"/>
       <c r="AC38" s="13"/>
       <c r="AD38" s="13"/>
@@ -11407,7 +11417,7 @@
       <c r="X39" s="13"/>
       <c r="Y39" s="13"/>
       <c r="Z39" s="13"/>
-      <c r="AA39" s="13"/>
+      <c r="AA39" s="34"/>
       <c r="AB39" s="13"/>
       <c r="AC39" s="13"/>
       <c r="AD39" s="13"/>
@@ -11441,7 +11451,7 @@
       <c r="X40" s="13"/>
       <c r="Y40" s="13"/>
       <c r="Z40" s="13"/>
-      <c r="AA40" s="13"/>
+      <c r="AA40" s="34"/>
       <c r="AB40" s="13"/>
       <c r="AC40" s="13"/>
       <c r="AD40" s="13"/>
@@ -11475,7 +11485,7 @@
       <c r="X41" s="13"/>
       <c r="Y41" s="13"/>
       <c r="Z41" s="13"/>
-      <c r="AA41" s="13"/>
+      <c r="AA41" s="34"/>
       <c r="AB41" s="13"/>
       <c r="AC41" s="13"/>
       <c r="AD41" s="13"/>
@@ -11509,7 +11519,7 @@
       <c r="X42" s="13"/>
       <c r="Y42" s="13"/>
       <c r="Z42" s="13"/>
-      <c r="AA42" s="13"/>
+      <c r="AA42" s="34"/>
       <c r="AB42" s="13"/>
       <c r="AC42" s="13"/>
       <c r="AD42" s="13"/>
@@ -11543,7 +11553,7 @@
       <c r="X43" s="13"/>
       <c r="Y43" s="13"/>
       <c r="Z43" s="13"/>
-      <c r="AA43" s="13"/>
+      <c r="AA43" s="34"/>
       <c r="AB43" s="13"/>
       <c r="AC43" s="13"/>
       <c r="AD43" s="13"/>
@@ -11577,7 +11587,7 @@
       <c r="X44" s="13"/>
       <c r="Y44" s="13"/>
       <c r="Z44" s="13"/>
-      <c r="AA44" s="13"/>
+      <c r="AA44" s="34"/>
       <c r="AB44" s="13"/>
       <c r="AC44" s="13"/>
       <c r="AD44" s="13"/>
@@ -11611,7 +11621,7 @@
       <c r="X45" s="13"/>
       <c r="Y45" s="13"/>
       <c r="Z45" s="13"/>
-      <c r="AA45" s="13"/>
+      <c r="AA45" s="34"/>
       <c r="AB45" s="13"/>
       <c r="AC45" s="13"/>
       <c r="AD45" s="13"/>
@@ -11645,7 +11655,7 @@
       <c r="X46" s="13"/>
       <c r="Y46" s="13"/>
       <c r="Z46" s="13"/>
-      <c r="AA46" s="13"/>
+      <c r="AA46" s="34"/>
       <c r="AB46" s="13"/>
       <c r="AC46" s="13"/>
       <c r="AD46" s="13"/>
@@ -11679,7 +11689,7 @@
       <c r="X47" s="13"/>
       <c r="Y47" s="13"/>
       <c r="Z47" s="13"/>
-      <c r="AA47" s="13"/>
+      <c r="AA47" s="34"/>
       <c r="AB47" s="13"/>
       <c r="AC47" s="13"/>
       <c r="AD47" s="13"/>
@@ -11713,7 +11723,7 @@
       <c r="X48" s="13"/>
       <c r="Y48" s="13"/>
       <c r="Z48" s="13"/>
-      <c r="AA48" s="13"/>
+      <c r="AA48" s="34"/>
       <c r="AB48" s="13"/>
       <c r="AC48" s="13"/>
       <c r="AD48" s="13"/>
@@ -11747,7 +11757,7 @@
       <c r="X49" s="13"/>
       <c r="Y49" s="13"/>
       <c r="Z49" s="13"/>
-      <c r="AA49" s="13"/>
+      <c r="AA49" s="34"/>
       <c r="AB49" s="13"/>
       <c r="AC49" s="13"/>
       <c r="AD49" s="13"/>
@@ -11781,7 +11791,7 @@
       <c r="X50" s="13"/>
       <c r="Y50" s="13"/>
       <c r="Z50" s="13"/>
-      <c r="AA50" s="13"/>
+      <c r="AA50" s="34"/>
       <c r="AB50" s="13"/>
       <c r="AC50" s="13"/>
       <c r="AD50" s="13"/>
@@ -11815,7 +11825,7 @@
       <c r="X51" s="13"/>
       <c r="Y51" s="13"/>
       <c r="Z51" s="13"/>
-      <c r="AA51" s="13"/>
+      <c r="AA51" s="34"/>
       <c r="AB51" s="13"/>
       <c r="AC51" s="13"/>
       <c r="AD51" s="13"/>
@@ -11849,7 +11859,7 @@
       <c r="X52" s="13"/>
       <c r="Y52" s="13"/>
       <c r="Z52" s="13"/>
-      <c r="AA52" s="13"/>
+      <c r="AA52" s="34"/>
       <c r="AB52" s="13"/>
       <c r="AC52" s="13"/>
       <c r="AD52" s="13"/>
@@ -11883,7 +11893,7 @@
       <c r="X53" s="13"/>
       <c r="Y53" s="13"/>
       <c r="Z53" s="13"/>
-      <c r="AA53" s="13"/>
+      <c r="AA53" s="34"/>
       <c r="AB53" s="13"/>
       <c r="AC53" s="13"/>
       <c r="AD53" s="13"/>
@@ -11917,7 +11927,7 @@
       <c r="X54" s="13"/>
       <c r="Y54" s="13"/>
       <c r="Z54" s="13"/>
-      <c r="AA54" s="13"/>
+      <c r="AA54" s="34"/>
       <c r="AB54" s="13"/>
       <c r="AC54" s="13"/>
       <c r="AD54" s="13"/>
@@ -11951,7 +11961,7 @@
       <c r="X55" s="13"/>
       <c r="Y55" s="13"/>
       <c r="Z55" s="13"/>
-      <c r="AA55" s="13"/>
+      <c r="AA55" s="34"/>
       <c r="AB55" s="13"/>
       <c r="AC55" s="13"/>
       <c r="AD55" s="13"/>
@@ -11985,7 +11995,7 @@
       <c r="X56" s="13"/>
       <c r="Y56" s="13"/>
       <c r="Z56" s="13"/>
-      <c r="AA56" s="13"/>
+      <c r="AA56" s="34"/>
       <c r="AB56" s="13"/>
       <c r="AC56" s="13"/>
       <c r="AD56" s="13"/>
@@ -12019,7 +12029,7 @@
       <c r="X57" s="13"/>
       <c r="Y57" s="13"/>
       <c r="Z57" s="13"/>
-      <c r="AA57" s="13"/>
+      <c r="AA57" s="34"/>
       <c r="AB57" s="13"/>
       <c r="AC57" s="13"/>
       <c r="AD57" s="13"/>
@@ -12053,7 +12063,7 @@
       <c r="X58" s="13"/>
       <c r="Y58" s="13"/>
       <c r="Z58" s="13"/>
-      <c r="AA58" s="13"/>
+      <c r="AA58" s="34"/>
       <c r="AB58" s="13"/>
       <c r="AC58" s="13"/>
       <c r="AD58" s="13"/>
@@ -12087,7 +12097,7 @@
       <c r="X59" s="13"/>
       <c r="Y59" s="13"/>
       <c r="Z59" s="13"/>
-      <c r="AA59" s="13"/>
+      <c r="AA59" s="34"/>
       <c r="AB59" s="13"/>
       <c r="AC59" s="13"/>
       <c r="AD59" s="13"/>
@@ -12121,7 +12131,7 @@
       <c r="X60" s="13"/>
       <c r="Y60" s="13"/>
       <c r="Z60" s="13"/>
-      <c r="AA60" s="13"/>
+      <c r="AA60" s="34"/>
       <c r="AB60" s="13"/>
       <c r="AC60" s="13"/>
       <c r="AD60" s="13"/>
@@ -12155,7 +12165,7 @@
       <c r="X61" s="13"/>
       <c r="Y61" s="13"/>
       <c r="Z61" s="13"/>
-      <c r="AA61" s="13"/>
+      <c r="AA61" s="34"/>
       <c r="AB61" s="13"/>
       <c r="AC61" s="13"/>
       <c r="AD61" s="13"/>
@@ -12189,7 +12199,7 @@
       <c r="X62" s="13"/>
       <c r="Y62" s="13"/>
       <c r="Z62" s="13"/>
-      <c r="AA62" s="13"/>
+      <c r="AA62" s="34"/>
       <c r="AB62" s="13"/>
       <c r="AC62" s="13"/>
       <c r="AD62" s="13"/>
@@ -12223,7 +12233,7 @@
       <c r="X63" s="13"/>
       <c r="Y63" s="13"/>
       <c r="Z63" s="13"/>
-      <c r="AA63" s="13"/>
+      <c r="AA63" s="34"/>
       <c r="AB63" s="13"/>
       <c r="AC63" s="13"/>
       <c r="AD63" s="13"/>
@@ -12257,7 +12267,7 @@
       <c r="X64" s="13"/>
       <c r="Y64" s="13"/>
       <c r="Z64" s="13"/>
-      <c r="AA64" s="13"/>
+      <c r="AA64" s="34"/>
       <c r="AB64" s="13"/>
       <c r="AC64" s="13"/>
       <c r="AD64" s="13"/>
@@ -12291,7 +12301,7 @@
       <c r="X65" s="13"/>
       <c r="Y65" s="13"/>
       <c r="Z65" s="13"/>
-      <c r="AA65" s="13"/>
+      <c r="AA65" s="34"/>
       <c r="AB65" s="13"/>
       <c r="AC65" s="13"/>
       <c r="AD65" s="13"/>
@@ -12325,7 +12335,7 @@
       <c r="X66" s="13"/>
       <c r="Y66" s="13"/>
       <c r="Z66" s="13"/>
-      <c r="AA66" s="13"/>
+      <c r="AA66" s="34"/>
       <c r="AB66" s="13"/>
       <c r="AC66" s="13"/>
       <c r="AD66" s="13"/>
@@ -12359,7 +12369,7 @@
       <c r="X67" s="13"/>
       <c r="Y67" s="13"/>
       <c r="Z67" s="13"/>
-      <c r="AA67" s="13"/>
+      <c r="AA67" s="34"/>
       <c r="AB67" s="13"/>
       <c r="AC67" s="13"/>
       <c r="AD67" s="13"/>
@@ -12393,7 +12403,7 @@
       <c r="X68" s="13"/>
       <c r="Y68" s="13"/>
       <c r="Z68" s="13"/>
-      <c r="AA68" s="13"/>
+      <c r="AA68" s="34"/>
       <c r="AB68" s="13"/>
       <c r="AC68" s="13"/>
       <c r="AD68" s="13"/>
@@ -12427,7 +12437,7 @@
       <c r="X69" s="13"/>
       <c r="Y69" s="13"/>
       <c r="Z69" s="13"/>
-      <c r="AA69" s="13"/>
+      <c r="AA69" s="34"/>
       <c r="AB69" s="13"/>
       <c r="AC69" s="13"/>
       <c r="AD69" s="13"/>
@@ -12461,7 +12471,7 @@
       <c r="X70" s="13"/>
       <c r="Y70" s="13"/>
       <c r="Z70" s="13"/>
-      <c r="AA70" s="13"/>
+      <c r="AA70" s="34"/>
       <c r="AB70" s="13"/>
       <c r="AC70" s="13"/>
       <c r="AD70" s="13"/>
@@ -12495,7 +12505,7 @@
       <c r="X71" s="13"/>
       <c r="Y71" s="13"/>
       <c r="Z71" s="13"/>
-      <c r="AA71" s="13"/>
+      <c r="AA71" s="34"/>
       <c r="AB71" s="13"/>
       <c r="AC71" s="13"/>
       <c r="AD71" s="13"/>
@@ -12529,7 +12539,7 @@
       <c r="X72" s="13"/>
       <c r="Y72" s="13"/>
       <c r="Z72" s="13"/>
-      <c r="AA72" s="13"/>
+      <c r="AA72" s="34"/>
       <c r="AB72" s="13"/>
       <c r="AC72" s="13"/>
       <c r="AD72" s="13"/>
@@ -12563,7 +12573,7 @@
       <c r="X73" s="13"/>
       <c r="Y73" s="13"/>
       <c r="Z73" s="13"/>
-      <c r="AA73" s="13"/>
+      <c r="AA73" s="34"/>
       <c r="AB73" s="13"/>
       <c r="AC73" s="13"/>
       <c r="AD73" s="13"/>
@@ -12597,7 +12607,7 @@
       <c r="X74" s="13"/>
       <c r="Y74" s="13"/>
       <c r="Z74" s="13"/>
-      <c r="AA74" s="13"/>
+      <c r="AA74" s="34"/>
       <c r="AB74" s="13"/>
       <c r="AC74" s="13"/>
       <c r="AD74" s="13"/>
@@ -12631,7 +12641,7 @@
       <c r="X75" s="13"/>
       <c r="Y75" s="13"/>
       <c r="Z75" s="13"/>
-      <c r="AA75" s="13"/>
+      <c r="AA75" s="34"/>
       <c r="AB75" s="13"/>
       <c r="AC75" s="13"/>
       <c r="AD75" s="13"/>
@@ -12665,7 +12675,7 @@
       <c r="X76" s="13"/>
       <c r="Y76" s="13"/>
       <c r="Z76" s="13"/>
-      <c r="AA76" s="13"/>
+      <c r="AA76" s="34"/>
       <c r="AB76" s="13"/>
       <c r="AC76" s="13"/>
       <c r="AD76" s="13"/>
@@ -12699,7 +12709,7 @@
       <c r="X77" s="13"/>
       <c r="Y77" s="13"/>
       <c r="Z77" s="13"/>
-      <c r="AA77" s="13"/>
+      <c r="AA77" s="34"/>
       <c r="AB77" s="13"/>
       <c r="AC77" s="13"/>
       <c r="AD77" s="13"/>
@@ -12733,7 +12743,7 @@
       <c r="X78" s="13"/>
       <c r="Y78" s="13"/>
       <c r="Z78" s="13"/>
-      <c r="AA78" s="13"/>
+      <c r="AA78" s="34"/>
       <c r="AB78" s="13"/>
       <c r="AC78" s="13"/>
       <c r="AD78" s="13"/>
@@ -12767,7 +12777,7 @@
       <c r="X79" s="13"/>
       <c r="Y79" s="13"/>
       <c r="Z79" s="13"/>
-      <c r="AA79" s="13"/>
+      <c r="AA79" s="34"/>
       <c r="AB79" s="13"/>
       <c r="AC79" s="13"/>
       <c r="AD79" s="13"/>
@@ -12801,7 +12811,7 @@
       <c r="X80" s="13"/>
       <c r="Y80" s="13"/>
       <c r="Z80" s="13"/>
-      <c r="AA80" s="13"/>
+      <c r="AA80" s="34"/>
       <c r="AB80" s="13"/>
       <c r="AC80" s="13"/>
       <c r="AD80" s="13"/>
@@ -12835,7 +12845,7 @@
       <c r="X81" s="13"/>
       <c r="Y81" s="13"/>
       <c r="Z81" s="13"/>
-      <c r="AA81" s="13"/>
+      <c r="AA81" s="34"/>
       <c r="AB81" s="13"/>
       <c r="AC81" s="13"/>
       <c r="AD81" s="13"/>
@@ -12869,7 +12879,7 @@
       <c r="X82" s="13"/>
       <c r="Y82" s="13"/>
       <c r="Z82" s="13"/>
-      <c r="AA82" s="13"/>
+      <c r="AA82" s="34"/>
       <c r="AB82" s="13"/>
       <c r="AC82" s="13"/>
       <c r="AD82" s="13"/>
@@ -12903,7 +12913,7 @@
       <c r="X83" s="13"/>
       <c r="Y83" s="13"/>
       <c r="Z83" s="13"/>
-      <c r="AA83" s="13"/>
+      <c r="AA83" s="34"/>
       <c r="AB83" s="13"/>
       <c r="AC83" s="13"/>
       <c r="AD83" s="13"/>
@@ -12937,7 +12947,7 @@
       <c r="X84" s="13"/>
       <c r="Y84" s="13"/>
       <c r="Z84" s="13"/>
-      <c r="AA84" s="13"/>
+      <c r="AA84" s="34"/>
       <c r="AB84" s="13"/>
       <c r="AC84" s="13"/>
       <c r="AD84" s="13"/>
@@ -12971,7 +12981,7 @@
       <c r="X85" s="13"/>
       <c r="Y85" s="13"/>
       <c r="Z85" s="13"/>
-      <c r="AA85" s="13"/>
+      <c r="AA85" s="34"/>
       <c r="AB85" s="13"/>
       <c r="AC85" s="13"/>
       <c r="AD85" s="13"/>
@@ -13005,7 +13015,7 @@
       <c r="X86" s="13"/>
       <c r="Y86" s="13"/>
       <c r="Z86" s="13"/>
-      <c r="AA86" s="13"/>
+      <c r="AA86" s="34"/>
       <c r="AB86" s="13"/>
       <c r="AC86" s="13"/>
       <c r="AD86" s="13"/>
@@ -13039,7 +13049,7 @@
       <c r="X87" s="13"/>
       <c r="Y87" s="13"/>
       <c r="Z87" s="13"/>
-      <c r="AA87" s="13"/>
+      <c r="AA87" s="34"/>
       <c r="AB87" s="13"/>
       <c r="AC87" s="13"/>
       <c r="AD87" s="13"/>
@@ -13073,7 +13083,7 @@
       <c r="X88" s="13"/>
       <c r="Y88" s="13"/>
       <c r="Z88" s="13"/>
-      <c r="AA88" s="13"/>
+      <c r="AA88" s="34"/>
       <c r="AB88" s="13"/>
       <c r="AC88" s="13"/>
       <c r="AD88" s="13"/>
@@ -13107,7 +13117,7 @@
       <c r="X89" s="13"/>
       <c r="Y89" s="13"/>
       <c r="Z89" s="13"/>
-      <c r="AA89" s="13"/>
+      <c r="AA89" s="34"/>
       <c r="AB89" s="13"/>
       <c r="AC89" s="13"/>
       <c r="AD89" s="13"/>
@@ -13141,7 +13151,7 @@
       <c r="X90" s="13"/>
       <c r="Y90" s="13"/>
       <c r="Z90" s="13"/>
-      <c r="AA90" s="13"/>
+      <c r="AA90" s="34"/>
       <c r="AB90" s="13"/>
       <c r="AC90" s="13"/>
       <c r="AD90" s="13"/>
@@ -13175,7 +13185,7 @@
       <c r="X91" s="13"/>
       <c r="Y91" s="13"/>
       <c r="Z91" s="13"/>
-      <c r="AA91" s="13"/>
+      <c r="AA91" s="34"/>
       <c r="AB91" s="13"/>
       <c r="AC91" s="13"/>
       <c r="AD91" s="13"/>
@@ -13209,7 +13219,7 @@
       <c r="X92" s="13"/>
       <c r="Y92" s="13"/>
       <c r="Z92" s="13"/>
-      <c r="AA92" s="13"/>
+      <c r="AA92" s="34"/>
       <c r="AB92" s="13"/>
       <c r="AC92" s="13"/>
       <c r="AD92" s="13"/>
@@ -13243,7 +13253,7 @@
       <c r="X93" s="13"/>
       <c r="Y93" s="13"/>
       <c r="Z93" s="13"/>
-      <c r="AA93" s="13"/>
+      <c r="AA93" s="34"/>
       <c r="AB93" s="13"/>
       <c r="AC93" s="13"/>
       <c r="AD93" s="13"/>
@@ -13277,7 +13287,7 @@
       <c r="X94" s="13"/>
       <c r="Y94" s="13"/>
       <c r="Z94" s="13"/>
-      <c r="AA94" s="13"/>
+      <c r="AA94" s="34"/>
       <c r="AB94" s="13"/>
       <c r="AC94" s="13"/>
       <c r="AD94" s="13"/>
@@ -13311,7 +13321,7 @@
       <c r="X95" s="13"/>
       <c r="Y95" s="13"/>
       <c r="Z95" s="13"/>
-      <c r="AA95" s="13"/>
+      <c r="AA95" s="34"/>
       <c r="AB95" s="13"/>
       <c r="AC95" s="13"/>
       <c r="AD95" s="13"/>
@@ -13345,7 +13355,7 @@
       <c r="X96" s="13"/>
       <c r="Y96" s="13"/>
       <c r="Z96" s="13"/>
-      <c r="AA96" s="13"/>
+      <c r="AA96" s="34"/>
       <c r="AB96" s="13"/>
       <c r="AC96" s="13"/>
       <c r="AD96" s="13"/>
@@ -13379,7 +13389,7 @@
       <c r="X97" s="13"/>
       <c r="Y97" s="13"/>
       <c r="Z97" s="13"/>
-      <c r="AA97" s="13"/>
+      <c r="AA97" s="34"/>
       <c r="AB97" s="13"/>
       <c r="AC97" s="13"/>
       <c r="AD97" s="13"/>
@@ -13413,7 +13423,7 @@
       <c r="X98" s="13"/>
       <c r="Y98" s="13"/>
       <c r="Z98" s="13"/>
-      <c r="AA98" s="13"/>
+      <c r="AA98" s="34"/>
       <c r="AB98" s="13"/>
       <c r="AC98" s="13"/>
       <c r="AD98" s="13"/>
@@ -13447,7 +13457,7 @@
       <c r="X99" s="13"/>
       <c r="Y99" s="13"/>
       <c r="Z99" s="13"/>
-      <c r="AA99" s="13"/>
+      <c r="AA99" s="34"/>
       <c r="AB99" s="13"/>
       <c r="AC99" s="13"/>
       <c r="AD99" s="13"/>
@@ -13481,7 +13491,7 @@
       <c r="X100" s="13"/>
       <c r="Y100" s="13"/>
       <c r="Z100" s="13"/>
-      <c r="AA100" s="13"/>
+      <c r="AA100" s="34"/>
       <c r="AB100" s="13"/>
       <c r="AC100" s="13"/>
       <c r="AD100" s="13"/>
@@ -13515,7 +13525,7 @@
       <c r="X101" s="13"/>
       <c r="Y101" s="13"/>
       <c r="Z101" s="13"/>
-      <c r="AA101" s="13"/>
+      <c r="AA101" s="34"/>
       <c r="AB101" s="13"/>
       <c r="AC101" s="13"/>
       <c r="AD101" s="13"/>
@@ -13549,7 +13559,7 @@
       <c r="X102" s="13"/>
       <c r="Y102" s="13"/>
       <c r="Z102" s="13"/>
-      <c r="AA102" s="13"/>
+      <c r="AA102" s="34"/>
       <c r="AB102" s="13"/>
       <c r="AC102" s="13"/>
       <c r="AD102" s="13"/>
@@ -13583,7 +13593,7 @@
       <c r="X103" s="13"/>
       <c r="Y103" s="13"/>
       <c r="Z103" s="13"/>
-      <c r="AA103" s="13"/>
+      <c r="AA103" s="34"/>
       <c r="AB103" s="13"/>
       <c r="AC103" s="13"/>
       <c r="AD103" s="13"/>
@@ -13617,7 +13627,7 @@
       <c r="X104" s="13"/>
       <c r="Y104" s="13"/>
       <c r="Z104" s="13"/>
-      <c r="AA104" s="13"/>
+      <c r="AA104" s="34"/>
       <c r="AB104" s="13"/>
       <c r="AC104" s="13"/>
       <c r="AD104" s="13"/>
@@ -13651,7 +13661,7 @@
       <c r="X105" s="13"/>
       <c r="Y105" s="13"/>
       <c r="Z105" s="13"/>
-      <c r="AA105" s="13"/>
+      <c r="AA105" s="34"/>
       <c r="AB105" s="13"/>
       <c r="AC105" s="13"/>
       <c r="AD105" s="13"/>
@@ -13685,7 +13695,7 @@
       <c r="X106" s="13"/>
       <c r="Y106" s="13"/>
       <c r="Z106" s="13"/>
-      <c r="AA106" s="13"/>
+      <c r="AA106" s="34"/>
       <c r="AB106" s="13"/>
       <c r="AC106" s="13"/>
       <c r="AD106" s="13"/>
@@ -13719,7 +13729,7 @@
       <c r="X107" s="13"/>
       <c r="Y107" s="13"/>
       <c r="Z107" s="13"/>
-      <c r="AA107" s="13"/>
+      <c r="AA107" s="34"/>
       <c r="AB107" s="13"/>
       <c r="AC107" s="13"/>
       <c r="AD107" s="13"/>
@@ -13753,7 +13763,7 @@
       <c r="X108" s="13"/>
       <c r="Y108" s="13"/>
       <c r="Z108" s="13"/>
-      <c r="AA108" s="13"/>
+      <c r="AA108" s="34"/>
       <c r="AB108" s="13"/>
       <c r="AC108" s="13"/>
       <c r="AD108" s="13"/>
@@ -13787,7 +13797,7 @@
       <c r="X109" s="13"/>
       <c r="Y109" s="13"/>
       <c r="Z109" s="13"/>
-      <c r="AA109" s="13"/>
+      <c r="AA109" s="34"/>
       <c r="AB109" s="13"/>
       <c r="AC109" s="13"/>
       <c r="AD109" s="13"/>
@@ -13821,7 +13831,7 @@
       <c r="X110" s="13"/>
       <c r="Y110" s="13"/>
       <c r="Z110" s="13"/>
-      <c r="AA110" s="13"/>
+      <c r="AA110" s="34"/>
       <c r="AB110" s="13"/>
       <c r="AC110" s="13"/>
       <c r="AD110" s="13"/>
@@ -13855,7 +13865,7 @@
       <c r="X111" s="13"/>
       <c r="Y111" s="13"/>
       <c r="Z111" s="13"/>
-      <c r="AA111" s="13"/>
+      <c r="AA111" s="34"/>
       <c r="AB111" s="13"/>
       <c r="AC111" s="13"/>
       <c r="AD111" s="13"/>
@@ -13889,7 +13899,7 @@
       <c r="X112" s="13"/>
       <c r="Y112" s="13"/>
       <c r="Z112" s="13"/>
-      <c r="AA112" s="13"/>
+      <c r="AA112" s="34"/>
       <c r="AB112" s="13"/>
       <c r="AC112" s="13"/>
       <c r="AD112" s="13"/>
@@ -13923,7 +13933,7 @@
       <c r="X113" s="13"/>
       <c r="Y113" s="13"/>
       <c r="Z113" s="13"/>
-      <c r="AA113" s="13"/>
+      <c r="AA113" s="34"/>
       <c r="AB113" s="13"/>
       <c r="AC113" s="13"/>
       <c r="AD113" s="13"/>
@@ -13957,7 +13967,7 @@
       <c r="X114" s="13"/>
       <c r="Y114" s="13"/>
       <c r="Z114" s="13"/>
-      <c r="AA114" s="13"/>
+      <c r="AA114" s="34"/>
       <c r="AB114" s="13"/>
       <c r="AC114" s="13"/>
       <c r="AD114" s="13"/>
@@ -13991,7 +14001,7 @@
       <c r="X115" s="13"/>
       <c r="Y115" s="13"/>
       <c r="Z115" s="13"/>
-      <c r="AA115" s="13"/>
+      <c r="AA115" s="34"/>
       <c r="AB115" s="13"/>
       <c r="AC115" s="13"/>
       <c r="AD115" s="13"/>
@@ -14025,7 +14035,7 @@
       <c r="X116" s="13"/>
       <c r="Y116" s="13"/>
       <c r="Z116" s="13"/>
-      <c r="AA116" s="13"/>
+      <c r="AA116" s="34"/>
       <c r="AB116" s="13"/>
       <c r="AC116" s="13"/>
       <c r="AD116" s="13"/>
@@ -14059,7 +14069,7 @@
       <c r="X117" s="13"/>
       <c r="Y117" s="13"/>
       <c r="Z117" s="13"/>
-      <c r="AA117" s="13"/>
+      <c r="AA117" s="34"/>
       <c r="AB117" s="13"/>
       <c r="AC117" s="13"/>
       <c r="AD117" s="13"/>
@@ -14093,7 +14103,7 @@
       <c r="X118" s="13"/>
       <c r="Y118" s="13"/>
       <c r="Z118" s="13"/>
-      <c r="AA118" s="13"/>
+      <c r="AA118" s="34"/>
       <c r="AB118" s="13"/>
       <c r="AC118" s="13"/>
       <c r="AD118" s="13"/>
@@ -14127,7 +14137,7 @@
       <c r="X119" s="13"/>
       <c r="Y119" s="13"/>
       <c r="Z119" s="13"/>
-      <c r="AA119" s="13"/>
+      <c r="AA119" s="34"/>
       <c r="AB119" s="13"/>
       <c r="AC119" s="13"/>
       <c r="AD119" s="13"/>
@@ -14161,7 +14171,7 @@
       <c r="X120" s="13"/>
       <c r="Y120" s="13"/>
       <c r="Z120" s="13"/>
-      <c r="AA120" s="13"/>
+      <c r="AA120" s="34"/>
       <c r="AB120" s="13"/>
       <c r="AC120" s="13"/>
       <c r="AD120" s="13"/>
@@ -14195,7 +14205,7 @@
       <c r="X121" s="13"/>
       <c r="Y121" s="13"/>
       <c r="Z121" s="13"/>
-      <c r="AA121" s="13"/>
+      <c r="AA121" s="34"/>
       <c r="AB121" s="13"/>
       <c r="AC121" s="13"/>
       <c r="AD121" s="13"/>
@@ -14229,7 +14239,7 @@
       <c r="X122" s="13"/>
       <c r="Y122" s="13"/>
       <c r="Z122" s="13"/>
-      <c r="AA122" s="13"/>
+      <c r="AA122" s="34"/>
       <c r="AB122" s="13"/>
       <c r="AC122" s="13"/>
       <c r="AD122" s="13"/>
@@ -14263,7 +14273,7 @@
       <c r="X123" s="13"/>
       <c r="Y123" s="13"/>
       <c r="Z123" s="13"/>
-      <c r="AA123" s="13"/>
+      <c r="AA123" s="34"/>
       <c r="AB123" s="13"/>
       <c r="AC123" s="13"/>
       <c r="AD123" s="13"/>
@@ -14297,7 +14307,7 @@
       <c r="X124" s="13"/>
       <c r="Y124" s="13"/>
       <c r="Z124" s="13"/>
-      <c r="AA124" s="13"/>
+      <c r="AA124" s="34"/>
       <c r="AB124" s="13"/>
       <c r="AC124" s="13"/>
       <c r="AD124" s="13"/>
@@ -14331,7 +14341,7 @@
       <c r="X125" s="13"/>
       <c r="Y125" s="13"/>
       <c r="Z125" s="13"/>
-      <c r="AA125" s="13"/>
+      <c r="AA125" s="34"/>
       <c r="AB125" s="13"/>
       <c r="AC125" s="13"/>
       <c r="AD125" s="13"/>
@@ -14365,7 +14375,7 @@
       <c r="X126" s="13"/>
       <c r="Y126" s="13"/>
       <c r="Z126" s="13"/>
-      <c r="AA126" s="13"/>
+      <c r="AA126" s="34"/>
       <c r="AB126" s="13"/>
       <c r="AC126" s="13"/>
       <c r="AD126" s="13"/>
@@ -14399,7 +14409,7 @@
       <c r="X127" s="13"/>
       <c r="Y127" s="13"/>
       <c r="Z127" s="13"/>
-      <c r="AA127" s="13"/>
+      <c r="AA127" s="34"/>
       <c r="AB127" s="13"/>
       <c r="AC127" s="13"/>
       <c r="AD127" s="13"/>
@@ -14433,7 +14443,7 @@
       <c r="X128" s="13"/>
       <c r="Y128" s="13"/>
       <c r="Z128" s="13"/>
-      <c r="AA128" s="13"/>
+      <c r="AA128" s="34"/>
       <c r="AB128" s="13"/>
       <c r="AC128" s="13"/>
       <c r="AD128" s="13"/>
@@ -14467,7 +14477,7 @@
       <c r="X129" s="13"/>
       <c r="Y129" s="13"/>
       <c r="Z129" s="13"/>
-      <c r="AA129" s="13"/>
+      <c r="AA129" s="34"/>
       <c r="AB129" s="13"/>
       <c r="AC129" s="13"/>
       <c r="AD129" s="13"/>
@@ -14501,7 +14511,7 @@
       <c r="X130" s="13"/>
       <c r="Y130" s="13"/>
       <c r="Z130" s="13"/>
-      <c r="AA130" s="13"/>
+      <c r="AA130" s="34"/>
       <c r="AB130" s="13"/>
       <c r="AC130" s="13"/>
       <c r="AD130" s="13"/>
@@ -14535,7 +14545,7 @@
       <c r="X131" s="13"/>
       <c r="Y131" s="13"/>
       <c r="Z131" s="13"/>
-      <c r="AA131" s="13"/>
+      <c r="AA131" s="34"/>
       <c r="AB131" s="13"/>
       <c r="AC131" s="13"/>
       <c r="AD131" s="13"/>
@@ -14569,7 +14579,7 @@
       <c r="X132" s="13"/>
       <c r="Y132" s="13"/>
       <c r="Z132" s="13"/>
-      <c r="AA132" s="13"/>
+      <c r="AA132" s="34"/>
       <c r="AB132" s="13"/>
       <c r="AC132" s="13"/>
       <c r="AD132" s="13"/>
@@ -14603,7 +14613,7 @@
       <c r="X133" s="13"/>
       <c r="Y133" s="13"/>
       <c r="Z133" s="13"/>
-      <c r="AA133" s="13"/>
+      <c r="AA133" s="34"/>
       <c r="AB133" s="13"/>
       <c r="AC133" s="13"/>
       <c r="AD133" s="13"/>
@@ -14637,7 +14647,7 @@
       <c r="X134" s="13"/>
       <c r="Y134" s="13"/>
       <c r="Z134" s="13"/>
-      <c r="AA134" s="13"/>
+      <c r="AA134" s="34"/>
       <c r="AB134" s="13"/>
       <c r="AC134" s="13"/>
       <c r="AD134" s="13"/>
@@ -14671,7 +14681,7 @@
       <c r="X135" s="13"/>
       <c r="Y135" s="13"/>
       <c r="Z135" s="13"/>
-      <c r="AA135" s="13"/>
+      <c r="AA135" s="34"/>
       <c r="AB135" s="13"/>
       <c r="AC135" s="13"/>
       <c r="AD135" s="13"/>
@@ -14705,7 +14715,7 @@
       <c r="X136" s="13"/>
       <c r="Y136" s="13"/>
       <c r="Z136" s="13"/>
-      <c r="AA136" s="13"/>
+      <c r="AA136" s="34"/>
       <c r="AB136" s="13"/>
       <c r="AC136" s="13"/>
       <c r="AD136" s="13"/>
@@ -14739,7 +14749,7 @@
       <c r="X137" s="13"/>
       <c r="Y137" s="13"/>
       <c r="Z137" s="13"/>
-      <c r="AA137" s="13"/>
+      <c r="AA137" s="34"/>
       <c r="AB137" s="13"/>
       <c r="AC137" s="13"/>
       <c r="AD137" s="13"/>
@@ -14773,7 +14783,7 @@
       <c r="X138" s="13"/>
       <c r="Y138" s="13"/>
       <c r="Z138" s="13"/>
-      <c r="AA138" s="13"/>
+      <c r="AA138" s="34"/>
       <c r="AB138" s="13"/>
       <c r="AC138" s="13"/>
       <c r="AD138" s="13"/>
@@ -14807,7 +14817,7 @@
       <c r="X139" s="13"/>
       <c r="Y139" s="13"/>
       <c r="Z139" s="13"/>
-      <c r="AA139" s="13"/>
+      <c r="AA139" s="34"/>
       <c r="AB139" s="13"/>
       <c r="AC139" s="13"/>
       <c r="AD139" s="13"/>
@@ -14841,7 +14851,7 @@
       <c r="X140" s="13"/>
       <c r="Y140" s="13"/>
       <c r="Z140" s="13"/>
-      <c r="AA140" s="13"/>
+      <c r="AA140" s="34"/>
       <c r="AB140" s="13"/>
       <c r="AC140" s="13"/>
       <c r="AD140" s="13"/>
@@ -14875,7 +14885,7 @@
       <c r="X141" s="13"/>
       <c r="Y141" s="13"/>
       <c r="Z141" s="13"/>
-      <c r="AA141" s="13"/>
+      <c r="AA141" s="34"/>
       <c r="AB141" s="13"/>
       <c r="AC141" s="13"/>
       <c r="AD141" s="13"/>
@@ -14909,7 +14919,7 @@
       <c r="X142" s="13"/>
       <c r="Y142" s="13"/>
       <c r="Z142" s="13"/>
-      <c r="AA142" s="13"/>
+      <c r="AA142" s="34"/>
       <c r="AB142" s="13"/>
       <c r="AC142" s="13"/>
       <c r="AD142" s="13"/>
@@ -14943,7 +14953,7 @@
       <c r="X143" s="13"/>
       <c r="Y143" s="13"/>
       <c r="Z143" s="13"/>
-      <c r="AA143" s="13"/>
+      <c r="AA143" s="34"/>
       <c r="AB143" s="13"/>
       <c r="AC143" s="13"/>
       <c r="AD143" s="13"/>
@@ -14977,7 +14987,7 @@
       <c r="X144" s="13"/>
       <c r="Y144" s="13"/>
       <c r="Z144" s="13"/>
-      <c r="AA144" s="13"/>
+      <c r="AA144" s="34"/>
       <c r="AB144" s="13"/>
       <c r="AC144" s="13"/>
       <c r="AD144" s="13"/>
@@ -15011,7 +15021,7 @@
       <c r="X145" s="13"/>
       <c r="Y145" s="13"/>
       <c r="Z145" s="13"/>
-      <c r="AA145" s="13"/>
+      <c r="AA145" s="34"/>
       <c r="AB145" s="13"/>
       <c r="AC145" s="13"/>
       <c r="AD145" s="13"/>
@@ -15045,7 +15055,7 @@
       <c r="X146" s="13"/>
       <c r="Y146" s="13"/>
       <c r="Z146" s="13"/>
-      <c r="AA146" s="13"/>
+      <c r="AA146" s="34"/>
       <c r="AB146" s="13"/>
       <c r="AC146" s="13"/>
       <c r="AD146" s="13"/>
@@ -15079,7 +15089,7 @@
       <c r="X147" s="13"/>
       <c r="Y147" s="13"/>
       <c r="Z147" s="13"/>
-      <c r="AA147" s="13"/>
+      <c r="AA147" s="34"/>
       <c r="AB147" s="13"/>
       <c r="AC147" s="13"/>
       <c r="AD147" s="13"/>
@@ -15113,7 +15123,7 @@
       <c r="X148" s="13"/>
       <c r="Y148" s="13"/>
       <c r="Z148" s="13"/>
-      <c r="AA148" s="13"/>
+      <c r="AA148" s="34"/>
       <c r="AB148" s="13"/>
       <c r="AC148" s="13"/>
       <c r="AD148" s="13"/>
@@ -15147,7 +15157,7 @@
       <c r="X149" s="13"/>
       <c r="Y149" s="13"/>
       <c r="Z149" s="13"/>
-      <c r="AA149" s="13"/>
+      <c r="AA149" s="34"/>
       <c r="AB149" s="13"/>
       <c r="AC149" s="13"/>
       <c r="AD149" s="13"/>
@@ -15181,7 +15191,7 @@
       <c r="X150" s="13"/>
       <c r="Y150" s="13"/>
       <c r="Z150" s="13"/>
-      <c r="AA150" s="13"/>
+      <c r="AA150" s="34"/>
       <c r="AB150" s="13"/>
       <c r="AC150" s="13"/>
       <c r="AD150" s="13"/>
@@ -15215,7 +15225,7 @@
       <c r="X151" s="13"/>
       <c r="Y151" s="13"/>
       <c r="Z151" s="13"/>
-      <c r="AA151" s="13"/>
+      <c r="AA151" s="34"/>
       <c r="AB151" s="13"/>
       <c r="AC151" s="13"/>
       <c r="AD151" s="13"/>
@@ -15249,7 +15259,7 @@
       <c r="X152" s="13"/>
       <c r="Y152" s="13"/>
       <c r="Z152" s="13"/>
-      <c r="AA152" s="13"/>
+      <c r="AA152" s="34"/>
       <c r="AB152" s="13"/>
       <c r="AC152" s="13"/>
       <c r="AD152" s="13"/>
@@ -15283,7 +15293,7 @@
       <c r="X153" s="13"/>
       <c r="Y153" s="13"/>
       <c r="Z153" s="13"/>
-      <c r="AA153" s="13"/>
+      <c r="AA153" s="34"/>
       <c r="AB153" s="13"/>
       <c r="AC153" s="13"/>
       <c r="AD153" s="13"/>
@@ -15317,7 +15327,7 @@
       <c r="X154" s="13"/>
       <c r="Y154" s="13"/>
       <c r="Z154" s="13"/>
-      <c r="AA154" s="13"/>
+      <c r="AA154" s="34"/>
       <c r="AB154" s="13"/>
       <c r="AC154" s="13"/>
       <c r="AD154" s="13"/>
@@ -15351,7 +15361,7 @@
       <c r="X155" s="13"/>
       <c r="Y155" s="13"/>
       <c r="Z155" s="13"/>
-      <c r="AA155" s="13"/>
+      <c r="AA155" s="34"/>
       <c r="AB155" s="13"/>
       <c r="AC155" s="13"/>
       <c r="AD155" s="13"/>
@@ -15385,7 +15395,7 @@
       <c r="X156" s="13"/>
       <c r="Y156" s="13"/>
       <c r="Z156" s="13"/>
-      <c r="AA156" s="13"/>
+      <c r="AA156" s="34"/>
       <c r="AB156" s="13"/>
       <c r="AC156" s="13"/>
       <c r="AD156" s="13"/>
@@ -15419,7 +15429,7 @@
       <c r="X157" s="13"/>
       <c r="Y157" s="13"/>
       <c r="Z157" s="13"/>
-      <c r="AA157" s="13"/>
+      <c r="AA157" s="34"/>
       <c r="AB157" s="13"/>
       <c r="AC157" s="13"/>
       <c r="AD157" s="13"/>
@@ -15453,7 +15463,7 @@
       <c r="X158" s="13"/>
       <c r="Y158" s="13"/>
       <c r="Z158" s="13"/>
-      <c r="AA158" s="13"/>
+      <c r="AA158" s="34"/>
       <c r="AB158" s="13"/>
       <c r="AC158" s="13"/>
       <c r="AD158" s="13"/>
@@ -15487,7 +15497,7 @@
       <c r="X159" s="13"/>
       <c r="Y159" s="13"/>
       <c r="Z159" s="13"/>
-      <c r="AA159" s="13"/>
+      <c r="AA159" s="34"/>
       <c r="AB159" s="13"/>
       <c r="AC159" s="13"/>
       <c r="AD159" s="13"/>
@@ -15521,7 +15531,7 @@
       <c r="X160" s="13"/>
       <c r="Y160" s="13"/>
       <c r="Z160" s="13"/>
-      <c r="AA160" s="13"/>
+      <c r="AA160" s="34"/>
       <c r="AB160" s="13"/>
       <c r="AC160" s="13"/>
       <c r="AD160" s="13"/>
@@ -15555,7 +15565,7 @@
       <c r="X161" s="13"/>
       <c r="Y161" s="13"/>
       <c r="Z161" s="13"/>
-      <c r="AA161" s="13"/>
+      <c r="AA161" s="34"/>
       <c r="AB161" s="13"/>
       <c r="AC161" s="13"/>
       <c r="AD161" s="13"/>
@@ -15589,7 +15599,7 @@
       <c r="X162" s="13"/>
       <c r="Y162" s="13"/>
       <c r="Z162" s="13"/>
-      <c r="AA162" s="13"/>
+      <c r="AA162" s="34"/>
       <c r="AB162" s="13"/>
       <c r="AC162" s="13"/>
       <c r="AD162" s="13"/>
@@ -15623,7 +15633,7 @@
       <c r="X163" s="13"/>
       <c r="Y163" s="13"/>
       <c r="Z163" s="13"/>
-      <c r="AA163" s="13"/>
+      <c r="AA163" s="34"/>
       <c r="AB163" s="13"/>
       <c r="AC163" s="13"/>
       <c r="AD163" s="13"/>
@@ -15657,7 +15667,7 @@
       <c r="X164" s="13"/>
       <c r="Y164" s="13"/>
       <c r="Z164" s="13"/>
-      <c r="AA164" s="13"/>
+      <c r="AA164" s="34"/>
       <c r="AB164" s="13"/>
       <c r="AC164" s="13"/>
       <c r="AD164" s="13"/>
@@ -15691,7 +15701,7 @@
       <c r="X165" s="13"/>
       <c r="Y165" s="13"/>
       <c r="Z165" s="13"/>
-      <c r="AA165" s="13"/>
+      <c r="AA165" s="34"/>
       <c r="AB165" s="13"/>
       <c r="AC165" s="13"/>
       <c r="AD165" s="13"/>
@@ -15725,7 +15735,7 @@
       <c r="X166" s="13"/>
       <c r="Y166" s="13"/>
       <c r="Z166" s="13"/>
-      <c r="AA166" s="13"/>
+      <c r="AA166" s="34"/>
       <c r="AB166" s="13"/>
       <c r="AC166" s="13"/>
       <c r="AD166" s="13"/>
@@ -15759,7 +15769,7 @@
       <c r="X167" s="13"/>
       <c r="Y167" s="13"/>
       <c r="Z167" s="13"/>
-      <c r="AA167" s="13"/>
+      <c r="AA167" s="34"/>
       <c r="AB167" s="13"/>
       <c r="AC167" s="13"/>
       <c r="AD167" s="13"/>
@@ -15793,7 +15803,7 @@
       <c r="X168" s="13"/>
       <c r="Y168" s="13"/>
       <c r="Z168" s="13"/>
-      <c r="AA168" s="13"/>
+      <c r="AA168" s="34"/>
       <c r="AB168" s="13"/>
       <c r="AC168" s="13"/>
       <c r="AD168" s="13"/>
@@ -15827,7 +15837,7 @@
       <c r="X169" s="13"/>
       <c r="Y169" s="13"/>
       <c r="Z169" s="13"/>
-      <c r="AA169" s="13"/>
+      <c r="AA169" s="34"/>
       <c r="AB169" s="13"/>
       <c r="AC169" s="13"/>
       <c r="AD169" s="13"/>
@@ -15861,7 +15871,7 @@
       <c r="X170" s="13"/>
       <c r="Y170" s="13"/>
       <c r="Z170" s="13"/>
-      <c r="AA170" s="13"/>
+      <c r="AA170" s="34"/>
       <c r="AB170" s="13"/>
       <c r="AC170" s="13"/>
       <c r="AD170" s="13"/>
@@ -15895,7 +15905,7 @@
       <c r="X171" s="13"/>
       <c r="Y171" s="13"/>
       <c r="Z171" s="13"/>
-      <c r="AA171" s="13"/>
+      <c r="AA171" s="34"/>
       <c r="AB171" s="13"/>
       <c r="AC171" s="13"/>
       <c r="AD171" s="13"/>
@@ -15929,7 +15939,7 @@
       <c r="X172" s="13"/>
       <c r="Y172" s="13"/>
       <c r="Z172" s="13"/>
-      <c r="AA172" s="13"/>
+      <c r="AA172" s="34"/>
       <c r="AB172" s="13"/>
       <c r="AC172" s="13"/>
       <c r="AD172" s="13"/>
@@ -15963,7 +15973,7 @@
       <c r="X173" s="13"/>
       <c r="Y173" s="13"/>
       <c r="Z173" s="13"/>
-      <c r="AA173" s="13"/>
+      <c r="AA173" s="34"/>
       <c r="AB173" s="13"/>
       <c r="AC173" s="13"/>
       <c r="AD173" s="13"/>
@@ -15997,7 +16007,7 @@
       <c r="X174" s="13"/>
       <c r="Y174" s="13"/>
       <c r="Z174" s="13"/>
-      <c r="AA174" s="13"/>
+      <c r="AA174" s="34"/>
       <c r="AB174" s="13"/>
       <c r="AC174" s="13"/>
       <c r="AD174" s="13"/>
@@ -16031,7 +16041,7 @@
       <c r="X175" s="13"/>
       <c r="Y175" s="13"/>
       <c r="Z175" s="13"/>
-      <c r="AA175" s="13"/>
+      <c r="AA175" s="34"/>
       <c r="AB175" s="13"/>
       <c r="AC175" s="13"/>
       <c r="AD175" s="13"/>
@@ -16065,7 +16075,7 @@
       <c r="X176" s="13"/>
       <c r="Y176" s="13"/>
       <c r="Z176" s="13"/>
-      <c r="AA176" s="13"/>
+      <c r="AA176" s="34"/>
       <c r="AB176" s="13"/>
       <c r="AC176" s="13"/>
       <c r="AD176" s="13"/>
@@ -16099,7 +16109,7 @@
       <c r="X177" s="13"/>
       <c r="Y177" s="13"/>
       <c r="Z177" s="13"/>
-      <c r="AA177" s="13"/>
+      <c r="AA177" s="34"/>
       <c r="AB177" s="13"/>
       <c r="AC177" s="13"/>
       <c r="AD177" s="13"/>
@@ -16133,7 +16143,7 @@
       <c r="X178" s="13"/>
       <c r="Y178" s="13"/>
       <c r="Z178" s="13"/>
-      <c r="AA178" s="13"/>
+      <c r="AA178" s="34"/>
       <c r="AB178" s="13"/>
       <c r="AC178" s="13"/>
       <c r="AD178" s="13"/>
@@ -16167,7 +16177,7 @@
       <c r="X179" s="13"/>
       <c r="Y179" s="13"/>
       <c r="Z179" s="13"/>
-      <c r="AA179" s="13"/>
+      <c r="AA179" s="34"/>
       <c r="AB179" s="13"/>
       <c r="AC179" s="13"/>
       <c r="AD179" s="13"/>
@@ -16201,7 +16211,7 @@
       <c r="X180" s="13"/>
       <c r="Y180" s="13"/>
       <c r="Z180" s="13"/>
-      <c r="AA180" s="13"/>
+      <c r="AA180" s="34"/>
       <c r="AB180" s="13"/>
       <c r="AC180" s="13"/>
       <c r="AD180" s="13"/>
@@ -16235,7 +16245,7 @@
       <c r="X181" s="13"/>
       <c r="Y181" s="13"/>
       <c r="Z181" s="13"/>
-      <c r="AA181" s="13"/>
+      <c r="AA181" s="34"/>
       <c r="AB181" s="13"/>
       <c r="AC181" s="13"/>
       <c r="AD181" s="13"/>
@@ -16269,7 +16279,7 @@
       <c r="X182" s="13"/>
       <c r="Y182" s="13"/>
       <c r="Z182" s="13"/>
-      <c r="AA182" s="13"/>
+      <c r="AA182" s="34"/>
       <c r="AB182" s="13"/>
       <c r="AC182" s="13"/>
       <c r="AD182" s="13"/>
@@ -16303,7 +16313,7 @@
       <c r="X183" s="13"/>
       <c r="Y183" s="13"/>
       <c r="Z183" s="13"/>
-      <c r="AA183" s="13"/>
+      <c r="AA183" s="34"/>
       <c r="AB183" s="13"/>
       <c r="AC183" s="13"/>
       <c r="AD183" s="13"/>
@@ -16337,7 +16347,7 @@
       <c r="X184" s="13"/>
       <c r="Y184" s="13"/>
       <c r="Z184" s="13"/>
-      <c r="AA184" s="13"/>
+      <c r="AA184" s="34"/>
       <c r="AB184" s="13"/>
       <c r="AC184" s="13"/>
       <c r="AD184" s="13"/>
@@ -16371,7 +16381,7 @@
       <c r="X185" s="13"/>
       <c r="Y185" s="13"/>
       <c r="Z185" s="13"/>
-      <c r="AA185" s="13"/>
+      <c r="AA185" s="34"/>
       <c r="AB185" s="13"/>
       <c r="AC185" s="13"/>
       <c r="AD185" s="13"/>
@@ -16405,7 +16415,7 @@
       <c r="X186" s="13"/>
       <c r="Y186" s="13"/>
       <c r="Z186" s="13"/>
-      <c r="AA186" s="13"/>
+      <c r="AA186" s="34"/>
       <c r="AB186" s="13"/>
       <c r="AC186" s="13"/>
       <c r="AD186" s="13"/>
@@ -16439,7 +16449,7 @@
       <c r="X187" s="13"/>
       <c r="Y187" s="13"/>
       <c r="Z187" s="13"/>
-      <c r="AA187" s="13"/>
+      <c r="AA187" s="34"/>
       <c r="AB187" s="13"/>
       <c r="AC187" s="13"/>
       <c r="AD187" s="13"/>
@@ -16473,7 +16483,7 @@
       <c r="X188" s="13"/>
       <c r="Y188" s="13"/>
       <c r="Z188" s="13"/>
-      <c r="AA188" s="13"/>
+      <c r="AA188" s="34"/>
       <c r="AB188" s="13"/>
       <c r="AC188" s="13"/>
       <c r="AD188" s="13"/>
@@ -16507,7 +16517,7 @@
       <c r="X189" s="13"/>
       <c r="Y189" s="13"/>
       <c r="Z189" s="13"/>
-      <c r="AA189" s="13"/>
+      <c r="AA189" s="34"/>
       <c r="AB189" s="13"/>
       <c r="AC189" s="13"/>
       <c r="AD189" s="13"/>
@@ -16541,7 +16551,7 @@
       <c r="X190" s="13"/>
       <c r="Y190" s="13"/>
       <c r="Z190" s="13"/>
-      <c r="AA190" s="13"/>
+      <c r="AA190" s="34"/>
       <c r="AB190" s="13"/>
       <c r="AC190" s="13"/>
       <c r="AD190" s="13"/>
@@ -16575,7 +16585,7 @@
       <c r="X191" s="13"/>
       <c r="Y191" s="13"/>
       <c r="Z191" s="13"/>
-      <c r="AA191" s="13"/>
+      <c r="AA191" s="34"/>
       <c r="AB191" s="13"/>
       <c r="AC191" s="13"/>
       <c r="AD191" s="13"/>
@@ -16609,7 +16619,7 @@
       <c r="X192" s="13"/>
       <c r="Y192" s="13"/>
       <c r="Z192" s="13"/>
-      <c r="AA192" s="13"/>
+      <c r="AA192" s="34"/>
       <c r="AB192" s="13"/>
       <c r="AC192" s="13"/>
       <c r="AD192" s="13"/>
@@ -16643,7 +16653,7 @@
       <c r="X193" s="13"/>
       <c r="Y193" s="13"/>
       <c r="Z193" s="13"/>
-      <c r="AA193" s="13"/>
+      <c r="AA193" s="34"/>
       <c r="AB193" s="13"/>
       <c r="AC193" s="13"/>
       <c r="AD193" s="13"/>
@@ -16677,7 +16687,7 @@
       <c r="X194" s="13"/>
       <c r="Y194" s="13"/>
       <c r="Z194" s="13"/>
-      <c r="AA194" s="13"/>
+      <c r="AA194" s="34"/>
       <c r="AB194" s="13"/>
       <c r="AC194" s="13"/>
       <c r="AD194" s="13"/>
@@ -16711,7 +16721,7 @@
       <c r="X195" s="13"/>
       <c r="Y195" s="13"/>
       <c r="Z195" s="13"/>
-      <c r="AA195" s="13"/>
+      <c r="AA195" s="34"/>
       <c r="AB195" s="13"/>
       <c r="AC195" s="13"/>
       <c r="AD195" s="13"/>
@@ -16745,7 +16755,7 @@
       <c r="X196" s="13"/>
       <c r="Y196" s="13"/>
       <c r="Z196" s="13"/>
-      <c r="AA196" s="13"/>
+      <c r="AA196" s="34"/>
       <c r="AB196" s="13"/>
       <c r="AC196" s="13"/>
       <c r="AD196" s="13"/>
@@ -16779,7 +16789,7 @@
       <c r="X197" s="13"/>
       <c r="Y197" s="13"/>
       <c r="Z197" s="13"/>
-      <c r="AA197" s="13"/>
+      <c r="AA197" s="34"/>
       <c r="AB197" s="13"/>
       <c r="AC197" s="13"/>
       <c r="AD197" s="13"/>
@@ -16813,7 +16823,7 @@
       <c r="X198" s="13"/>
       <c r="Y198" s="13"/>
       <c r="Z198" s="13"/>
-      <c r="AA198" s="13"/>
+      <c r="AA198" s="34"/>
       <c r="AB198" s="13"/>
       <c r="AC198" s="13"/>
       <c r="AD198" s="13"/>
@@ -16847,7 +16857,7 @@
       <c r="X199" s="13"/>
       <c r="Y199" s="13"/>
       <c r="Z199" s="13"/>
-      <c r="AA199" s="13"/>
+      <c r="AA199" s="34"/>
       <c r="AB199" s="13"/>
       <c r="AC199" s="13"/>
       <c r="AD199" s="13"/>
@@ -16881,7 +16891,7 @@
       <c r="X200" s="13"/>
       <c r="Y200" s="13"/>
       <c r="Z200" s="13"/>
-      <c r="AA200" s="13"/>
+      <c r="AA200" s="34"/>
       <c r="AB200" s="13"/>
       <c r="AC200" s="13"/>
       <c r="AD200" s="13"/>
@@ -16915,7 +16925,7 @@
       <c r="X201" s="13"/>
       <c r="Y201" s="13"/>
       <c r="Z201" s="13"/>
-      <c r="AA201" s="13"/>
+      <c r="AA201" s="34"/>
       <c r="AB201" s="13"/>
       <c r="AC201" s="13"/>
       <c r="AD201" s="13"/>
@@ -16949,7 +16959,7 @@
       <c r="X202" s="13"/>
       <c r="Y202" s="13"/>
       <c r="Z202" s="13"/>
-      <c r="AA202" s="13"/>
+      <c r="AA202" s="34"/>
       <c r="AB202" s="13"/>
       <c r="AC202" s="13"/>
       <c r="AD202" s="13"/>
@@ -16983,7 +16993,7 @@
       <c r="X203" s="13"/>
       <c r="Y203" s="13"/>
       <c r="Z203" s="13"/>
-      <c r="AA203" s="13"/>
+      <c r="AA203" s="34"/>
       <c r="AB203" s="13"/>
       <c r="AC203" s="13"/>
       <c r="AD203" s="13"/>
@@ -17017,7 +17027,7 @@
       <c r="X204" s="13"/>
       <c r="Y204" s="13"/>
       <c r="Z204" s="13"/>
-      <c r="AA204" s="13"/>
+      <c r="AA204" s="34"/>
       <c r="AB204" s="13"/>
       <c r="AC204" s="13"/>
       <c r="AD204" s="13"/>
@@ -17051,7 +17061,7 @@
       <c r="X205" s="13"/>
       <c r="Y205" s="13"/>
       <c r="Z205" s="13"/>
-      <c r="AA205" s="13"/>
+      <c r="AA205" s="34"/>
       <c r="AB205" s="13"/>
       <c r="AC205" s="13"/>
       <c r="AD205" s="13"/>
@@ -17085,7 +17095,7 @@
       <c r="X206" s="13"/>
       <c r="Y206" s="13"/>
       <c r="Z206" s="13"/>
-      <c r="AA206" s="13"/>
+      <c r="AA206" s="34"/>
       <c r="AB206" s="13"/>
       <c r="AC206" s="13"/>
       <c r="AD206" s="13"/>
@@ -17119,7 +17129,7 @@
       <c r="X207" s="13"/>
       <c r="Y207" s="13"/>
       <c r="Z207" s="13"/>
-      <c r="AA207" s="13"/>
+      <c r="AA207" s="34"/>
       <c r="AB207" s="13"/>
       <c r="AC207" s="13"/>
       <c r="AD207" s="13"/>
@@ -17153,7 +17163,7 @@
       <c r="X208" s="13"/>
       <c r="Y208" s="13"/>
       <c r="Z208" s="13"/>
-      <c r="AA208" s="13"/>
+      <c r="AA208" s="34"/>
       <c r="AB208" s="13"/>
       <c r="AC208" s="13"/>
       <c r="AD208" s="13"/>
@@ -17187,7 +17197,7 @@
       <c r="X209" s="13"/>
       <c r="Y209" s="13"/>
       <c r="Z209" s="13"/>
-      <c r="AA209" s="13"/>
+      <c r="AA209" s="34"/>
       <c r="AB209" s="13"/>
       <c r="AC209" s="13"/>
       <c r="AD209" s="13"/>
@@ -17221,7 +17231,7 @@
       <c r="X210" s="13"/>
       <c r="Y210" s="13"/>
       <c r="Z210" s="13"/>
-      <c r="AA210" s="13"/>
+      <c r="AA210" s="34"/>
       <c r="AB210" s="13"/>
       <c r="AC210" s="13"/>
       <c r="AD210" s="13"/>
@@ -17255,7 +17265,7 @@
       <c r="X211" s="13"/>
       <c r="Y211" s="13"/>
       <c r="Z211" s="13"/>
-      <c r="AA211" s="13"/>
+      <c r="AA211" s="34"/>
       <c r="AB211" s="13"/>
       <c r="AC211" s="13"/>
       <c r="AD211" s="13"/>
@@ -17289,7 +17299,7 @@
       <c r="X212" s="13"/>
       <c r="Y212" s="13"/>
       <c r="Z212" s="13"/>
-      <c r="AA212" s="13"/>
+      <c r="AA212" s="34"/>
       <c r="AB212" s="13"/>
       <c r="AC212" s="13"/>
       <c r="AD212" s="13"/>
@@ -17323,7 +17333,7 @@
       <c r="X213" s="13"/>
       <c r="Y213" s="13"/>
       <c r="Z213" s="13"/>
-      <c r="AA213" s="13"/>
+      <c r="AA213" s="34"/>
       <c r="AB213" s="13"/>
       <c r="AC213" s="13"/>
       <c r="AD213" s="13"/>
@@ -17357,7 +17367,7 @@
       <c r="X214" s="13"/>
       <c r="Y214" s="13"/>
       <c r="Z214" s="13"/>
-      <c r="AA214" s="13"/>
+      <c r="AA214" s="34"/>
       <c r="AB214" s="13"/>
       <c r="AC214" s="13"/>
       <c r="AD214" s="13"/>
@@ -17391,7 +17401,7 @@
       <c r="X215" s="13"/>
       <c r="Y215" s="13"/>
       <c r="Z215" s="13"/>
-      <c r="AA215" s="13"/>
+      <c r="AA215" s="34"/>
       <c r="AB215" s="13"/>
       <c r="AC215" s="13"/>
       <c r="AD215" s="13"/>
@@ -17425,7 +17435,7 @@
       <c r="X216" s="13"/>
       <c r="Y216" s="13"/>
       <c r="Z216" s="13"/>
-      <c r="AA216" s="13"/>
+      <c r="AA216" s="34"/>
       <c r="AB216" s="13"/>
       <c r="AC216" s="13"/>
       <c r="AD216" s="13"/>
@@ -17459,7 +17469,7 @@
       <c r="X217" s="13"/>
       <c r="Y217" s="13"/>
       <c r="Z217" s="13"/>
-      <c r="AA217" s="13"/>
+      <c r="AA217" s="34"/>
       <c r="AB217" s="13"/>
       <c r="AC217" s="13"/>
       <c r="AD217" s="13"/>
@@ -17493,7 +17503,7 @@
       <c r="X218" s="13"/>
       <c r="Y218" s="13"/>
       <c r="Z218" s="13"/>
-      <c r="AA218" s="13"/>
+      <c r="AA218" s="34"/>
       <c r="AB218" s="13"/>
       <c r="AC218" s="13"/>
       <c r="AD218" s="13"/>
@@ -17527,7 +17537,7 @@
       <c r="X219" s="13"/>
       <c r="Y219" s="13"/>
       <c r="Z219" s="13"/>
-      <c r="AA219" s="13"/>
+      <c r="AA219" s="34"/>
       <c r="AB219" s="13"/>
       <c r="AC219" s="13"/>
       <c r="AD219" s="13"/>
@@ -17561,7 +17571,7 @@
       <c r="X220" s="13"/>
       <c r="Y220" s="13"/>
       <c r="Z220" s="13"/>
-      <c r="AA220" s="13"/>
+      <c r="AA220" s="34"/>
       <c r="AB220" s="13"/>
       <c r="AC220" s="13"/>
       <c r="AD220" s="13"/>
@@ -17595,7 +17605,7 @@
       <c r="X221" s="13"/>
       <c r="Y221" s="13"/>
       <c r="Z221" s="13"/>
-      <c r="AA221" s="13"/>
+      <c r="AA221" s="34"/>
       <c r="AB221" s="13"/>
       <c r="AC221" s="13"/>
       <c r="AD221" s="13"/>
@@ -17629,7 +17639,7 @@
       <c r="X222" s="13"/>
       <c r="Y222" s="13"/>
       <c r="Z222" s="13"/>
-      <c r="AA222" s="13"/>
+      <c r="AA222" s="34"/>
       <c r="AB222" s="13"/>
       <c r="AC222" s="13"/>
       <c r="AD222" s="13"/>
@@ -17663,7 +17673,7 @@
       <c r="X223" s="13"/>
       <c r="Y223" s="13"/>
       <c r="Z223" s="13"/>
-      <c r="AA223" s="13"/>
+      <c r="AA223" s="34"/>
       <c r="AB223" s="13"/>
       <c r="AC223" s="13"/>
       <c r="AD223" s="13"/>
@@ -17697,7 +17707,7 @@
       <c r="X224" s="13"/>
       <c r="Y224" s="13"/>
       <c r="Z224" s="13"/>
-      <c r="AA224" s="13"/>
+      <c r="AA224" s="34"/>
       <c r="AB224" s="13"/>
       <c r="AC224" s="13"/>
       <c r="AD224" s="13"/>
@@ -17731,7 +17741,7 @@
       <c r="X225" s="13"/>
       <c r="Y225" s="13"/>
       <c r="Z225" s="13"/>
-      <c r="AA225" s="13"/>
+      <c r="AA225" s="34"/>
       <c r="AB225" s="13"/>
       <c r="AC225" s="13"/>
       <c r="AD225" s="13"/>
@@ -17765,7 +17775,7 @@
       <c r="X226" s="13"/>
       <c r="Y226" s="13"/>
       <c r="Z226" s="13"/>
-      <c r="AA226" s="13"/>
+      <c r="AA226" s="34"/>
       <c r="AB226" s="13"/>
       <c r="AC226" s="13"/>
       <c r="AD226" s="13"/>
@@ -17799,7 +17809,7 @@
       <c r="X227" s="13"/>
       <c r="Y227" s="13"/>
       <c r="Z227" s="13"/>
-      <c r="AA227" s="13"/>
+      <c r="AA227" s="34"/>
       <c r="AB227" s="13"/>
       <c r="AC227" s="13"/>
       <c r="AD227" s="13"/>
@@ -17833,7 +17843,7 @@
       <c r="X228" s="13"/>
       <c r="Y228" s="13"/>
       <c r="Z228" s="13"/>
-      <c r="AA228" s="13"/>
+      <c r="AA228" s="34"/>
       <c r="AB228" s="13"/>
       <c r="AC228" s="13"/>
       <c r="AD228" s="13"/>
@@ -17867,7 +17877,7 @@
       <c r="X229" s="13"/>
       <c r="Y229" s="13"/>
       <c r="Z229" s="13"/>
-      <c r="AA229" s="13"/>
+      <c r="AA229" s="34"/>
       <c r="AB229" s="13"/>
       <c r="AC229" s="13"/>
       <c r="AD229" s="13"/>
@@ -17901,7 +17911,7 @@
       <c r="X230" s="13"/>
       <c r="Y230" s="13"/>
       <c r="Z230" s="13"/>
-      <c r="AA230" s="13"/>
+      <c r="AA230" s="34"/>
       <c r="AB230" s="13"/>
       <c r="AC230" s="13"/>
       <c r="AD230" s="13"/>
@@ -17935,7 +17945,7 @@
       <c r="X231" s="13"/>
       <c r="Y231" s="13"/>
       <c r="Z231" s="13"/>
-      <c r="AA231" s="13"/>
+      <c r="AA231" s="34"/>
       <c r="AB231" s="13"/>
       <c r="AC231" s="13"/>
       <c r="AD231" s="13"/>
@@ -17969,7 +17979,7 @@
       <c r="X232" s="13"/>
       <c r="Y232" s="13"/>
       <c r="Z232" s="13"/>
-      <c r="AA232" s="13"/>
+      <c r="AA232" s="34"/>
       <c r="AB232" s="13"/>
       <c r="AC232" s="13"/>
       <c r="AD232" s="13"/>
@@ -18003,7 +18013,7 @@
       <c r="X233" s="13"/>
       <c r="Y233" s="13"/>
       <c r="Z233" s="13"/>
-      <c r="AA233" s="13"/>
+      <c r="AA233" s="34"/>
       <c r="AB233" s="13"/>
       <c r="AC233" s="13"/>
       <c r="AD233" s="13"/>
@@ -18037,7 +18047,7 @@
       <c r="X234" s="13"/>
       <c r="Y234" s="13"/>
       <c r="Z234" s="13"/>
-      <c r="AA234" s="13"/>
+      <c r="AA234" s="34"/>
       <c r="AB234" s="13"/>
       <c r="AC234" s="13"/>
       <c r="AD234" s="13"/>
@@ -18071,7 +18081,7 @@
       <c r="X235" s="13"/>
       <c r="Y235" s="13"/>
       <c r="Z235" s="13"/>
-      <c r="AA235" s="13"/>
+      <c r="AA235" s="34"/>
       <c r="AB235" s="13"/>
       <c r="AC235" s="13"/>
       <c r="AD235" s="13"/>
@@ -18105,7 +18115,7 @@
       <c r="X236" s="13"/>
       <c r="Y236" s="13"/>
       <c r="Z236" s="13"/>
-      <c r="AA236" s="13"/>
+      <c r="AA236" s="34"/>
       <c r="AB236" s="13"/>
       <c r="AC236" s="13"/>
       <c r="AD236" s="13"/>
@@ -18139,7 +18149,7 @@
       <c r="X237" s="13"/>
       <c r="Y237" s="13"/>
       <c r="Z237" s="13"/>
-      <c r="AA237" s="13"/>
+      <c r="AA237" s="34"/>
       <c r="AB237" s="13"/>
       <c r="AC237" s="13"/>
       <c r="AD237" s="13"/>
@@ -18173,7 +18183,7 @@
       <c r="X238" s="13"/>
       <c r="Y238" s="13"/>
       <c r="Z238" s="13"/>
-      <c r="AA238" s="13"/>
+      <c r="AA238" s="34"/>
       <c r="AB238" s="13"/>
       <c r="AC238" s="13"/>
       <c r="AD238" s="13"/>
@@ -18207,7 +18217,7 @@
       <c r="X239" s="13"/>
       <c r="Y239" s="13"/>
       <c r="Z239" s="13"/>
-      <c r="AA239" s="13"/>
+      <c r="AA239" s="34"/>
       <c r="AB239" s="13"/>
       <c r="AC239" s="13"/>
       <c r="AD239" s="13"/>
@@ -18241,7 +18251,7 @@
       <c r="X240" s="13"/>
       <c r="Y240" s="13"/>
       <c r="Z240" s="13"/>
-      <c r="AA240" s="13"/>
+      <c r="AA240" s="34"/>
       <c r="AB240" s="13"/>
       <c r="AC240" s="13"/>
       <c r="AD240" s="13"/>
@@ -18275,7 +18285,7 @@
       <c r="X241" s="13"/>
       <c r="Y241" s="13"/>
       <c r="Z241" s="13"/>
-      <c r="AA241" s="13"/>
+      <c r="AA241" s="34"/>
       <c r="AB241" s="13"/>
       <c r="AC241" s="13"/>
       <c r="AD241" s="13"/>
@@ -18309,7 +18319,7 @@
       <c r="X242" s="13"/>
       <c r="Y242" s="13"/>
       <c r="Z242" s="13"/>
-      <c r="AA242" s="13"/>
+      <c r="AA242" s="34"/>
       <c r="AB242" s="13"/>
       <c r="AC242" s="13"/>
       <c r="AD242" s="13"/>
@@ -18343,7 +18353,7 @@
       <c r="X243" s="13"/>
       <c r="Y243" s="13"/>
       <c r="Z243" s="13"/>
-      <c r="AA243" s="13"/>
+      <c r="AA243" s="34"/>
       <c r="AB243" s="13"/>
       <c r="AC243" s="13"/>
       <c r="AD243" s="13"/>
@@ -18377,7 +18387,7 @@
       <c r="X244" s="13"/>
       <c r="Y244" s="13"/>
       <c r="Z244" s="13"/>
-      <c r="AA244" s="13"/>
+      <c r="AA244" s="34"/>
       <c r="AB244" s="13"/>
       <c r="AC244" s="13"/>
       <c r="AD244" s="13"/>
@@ -18411,7 +18421,7 @@
       <c r="X245" s="13"/>
       <c r="Y245" s="13"/>
       <c r="Z245" s="13"/>
-      <c r="AA245" s="13"/>
+      <c r="AA245" s="34"/>
       <c r="AB245" s="13"/>
       <c r="AC245" s="13"/>
       <c r="AD245" s="13"/>
@@ -18445,7 +18455,7 @@
       <c r="X246" s="13"/>
       <c r="Y246" s="13"/>
       <c r="Z246" s="13"/>
-      <c r="AA246" s="13"/>
+      <c r="AA246" s="34"/>
       <c r="AB246" s="13"/>
       <c r="AC246" s="13"/>
       <c r="AD246" s="13"/>
@@ -18479,7 +18489,7 @@
       <c r="X247" s="13"/>
       <c r="Y247" s="13"/>
       <c r="Z247" s="13"/>
-      <c r="AA247" s="13"/>
+      <c r="AA247" s="34"/>
       <c r="AB247" s="13"/>
       <c r="AC247" s="13"/>
       <c r="AD247" s="13"/>
@@ -18513,7 +18523,7 @@
       <c r="X248" s="13"/>
       <c r="Y248" s="13"/>
       <c r="Z248" s="13"/>
-      <c r="AA248" s="13"/>
+      <c r="AA248" s="34"/>
       <c r="AB248" s="13"/>
       <c r="AC248" s="13"/>
       <c r="AD248" s="13"/>
@@ -18547,7 +18557,7 @@
       <c r="X249" s="13"/>
       <c r="Y249" s="13"/>
       <c r="Z249" s="13"/>
-      <c r="AA249" s="13"/>
+      <c r="AA249" s="34"/>
       <c r="AB249" s="13"/>
       <c r="AC249" s="13"/>
       <c r="AD249" s="13"/>
@@ -18581,7 +18591,7 @@
       <c r="X250" s="13"/>
       <c r="Y250" s="13"/>
       <c r="Z250" s="13"/>
-      <c r="AA250" s="13"/>
+      <c r="AA250" s="34"/>
       <c r="AB250" s="13"/>
       <c r="AC250" s="13"/>
       <c r="AD250" s="13"/>
@@ -18615,7 +18625,7 @@
       <c r="X251" s="13"/>
       <c r="Y251" s="13"/>
       <c r="Z251" s="13"/>
-      <c r="AA251" s="13"/>
+      <c r="AA251" s="34"/>
       <c r="AB251" s="13"/>
       <c r="AC251" s="13"/>
       <c r="AD251" s="13"/>
@@ -18649,7 +18659,7 @@
       <c r="X252" s="13"/>
       <c r="Y252" s="13"/>
       <c r="Z252" s="13"/>
-      <c r="AA252" s="13"/>
+      <c r="AA252" s="34"/>
       <c r="AB252" s="13"/>
       <c r="AC252" s="13"/>
       <c r="AD252" s="13"/>
@@ -18683,7 +18693,7 @@
       <c r="X253" s="13"/>
       <c r="Y253" s="13"/>
       <c r="Z253" s="13"/>
-      <c r="AA253" s="13"/>
+      <c r="AA253" s="34"/>
       <c r="AB253" s="13"/>
       <c r="AC253" s="13"/>
       <c r="AD253" s="13"/>
@@ -18717,7 +18727,7 @@
       <c r="X254" s="13"/>
       <c r="Y254" s="13"/>
       <c r="Z254" s="13"/>
-      <c r="AA254" s="13"/>
+      <c r="AA254" s="34"/>
       <c r="AB254" s="13"/>
       <c r="AC254" s="13"/>
       <c r="AD254" s="13"/>
@@ -18751,7 +18761,7 @@
       <c r="X255" s="13"/>
       <c r="Y255" s="13"/>
       <c r="Z255" s="13"/>
-      <c r="AA255" s="13"/>
+      <c r="AA255" s="34"/>
       <c r="AB255" s="13"/>
       <c r="AC255" s="13"/>
       <c r="AD255" s="13"/>
@@ -18785,7 +18795,7 @@
       <c r="X256" s="13"/>
       <c r="Y256" s="13"/>
       <c r="Z256" s="13"/>
-      <c r="AA256" s="13"/>
+      <c r="AA256" s="34"/>
       <c r="AB256" s="13"/>
       <c r="AC256" s="13"/>
       <c r="AD256" s="13"/>
@@ -18819,7 +18829,7 @@
       <c r="X257" s="13"/>
       <c r="Y257" s="13"/>
       <c r="Z257" s="13"/>
-      <c r="AA257" s="13"/>
+      <c r="AA257" s="34"/>
       <c r="AB257" s="13"/>
       <c r="AC257" s="13"/>
       <c r="AD257" s="13"/>
@@ -18853,7 +18863,7 @@
       <c r="X258" s="13"/>
       <c r="Y258" s="13"/>
       <c r="Z258" s="13"/>
-      <c r="AA258" s="13"/>
+      <c r="AA258" s="34"/>
       <c r="AB258" s="13"/>
       <c r="AC258" s="13"/>
       <c r="AD258" s="13"/>
@@ -18887,7 +18897,7 @@
       <c r="X259" s="13"/>
       <c r="Y259" s="13"/>
       <c r="Z259" s="13"/>
-      <c r="AA259" s="13"/>
+      <c r="AA259" s="34"/>
       <c r="AB259" s="13"/>
       <c r="AC259" s="13"/>
       <c r="AD259" s="13"/>
@@ -18921,7 +18931,7 @@
       <c r="X260" s="13"/>
       <c r="Y260" s="13"/>
       <c r="Z260" s="13"/>
-      <c r="AA260" s="13"/>
+      <c r="AA260" s="34"/>
       <c r="AB260" s="13"/>
       <c r="AC260" s="13"/>
       <c r="AD260" s="13"/>
@@ -18955,7 +18965,7 @@
       <c r="X261" s="13"/>
       <c r="Y261" s="13"/>
       <c r="Z261" s="13"/>
-      <c r="AA261" s="13"/>
+      <c r="AA261" s="34"/>
       <c r="AB261" s="13"/>
       <c r="AC261" s="13"/>
       <c r="AD261" s="13"/>
@@ -18989,7 +18999,7 @@
       <c r="X262" s="13"/>
       <c r="Y262" s="13"/>
       <c r="Z262" s="13"/>
-      <c r="AA262" s="13"/>
+      <c r="AA262" s="34"/>
       <c r="AB262" s="13"/>
       <c r="AC262" s="13"/>
       <c r="AD262" s="13"/>
@@ -19023,7 +19033,7 @@
       <c r="X263" s="13"/>
       <c r="Y263" s="13"/>
       <c r="Z263" s="13"/>
-      <c r="AA263" s="13"/>
+      <c r="AA263" s="34"/>
       <c r="AB263" s="13"/>
       <c r="AC263" s="13"/>
       <c r="AD263" s="13"/>
@@ -19057,7 +19067,7 @@
       <c r="X264" s="13"/>
       <c r="Y264" s="13"/>
       <c r="Z264" s="13"/>
-      <c r="AA264" s="13"/>
+      <c r="AA264" s="34"/>
       <c r="AB264" s="13"/>
       <c r="AC264" s="13"/>
       <c r="AD264" s="13"/>
@@ -19091,7 +19101,7 @@
       <c r="X265" s="13"/>
       <c r="Y265" s="13"/>
       <c r="Z265" s="13"/>
-      <c r="AA265" s="13"/>
+      <c r="AA265" s="34"/>
       <c r="AB265" s="13"/>
       <c r="AC265" s="13"/>
       <c r="AD265" s="13"/>
@@ -19125,7 +19135,7 @@
       <c r="X266" s="13"/>
       <c r="Y266" s="13"/>
       <c r="Z266" s="13"/>
-      <c r="AA266" s="13"/>
+      <c r="AA266" s="34"/>
       <c r="AB266" s="13"/>
       <c r="AC266" s="13"/>
       <c r="AD266" s="13"/>
@@ -19159,7 +19169,7 @@
       <c r="X267" s="13"/>
       <c r="Y267" s="13"/>
       <c r="Z267" s="13"/>
-      <c r="AA267" s="13"/>
+      <c r="AA267" s="34"/>
       <c r="AB267" s="13"/>
       <c r="AC267" s="13"/>
       <c r="AD267" s="13"/>
@@ -19193,7 +19203,7 @@
       <c r="X268" s="13"/>
       <c r="Y268" s="13"/>
       <c r="Z268" s="13"/>
-      <c r="AA268" s="13"/>
+      <c r="AA268" s="34"/>
       <c r="AB268" s="13"/>
       <c r="AC268" s="13"/>
       <c r="AD268" s="13"/>
@@ -19227,7 +19237,7 @@
       <c r="X269" s="13"/>
       <c r="Y269" s="13"/>
       <c r="Z269" s="13"/>
-      <c r="AA269" s="13"/>
+      <c r="AA269" s="34"/>
       <c r="AB269" s="13"/>
       <c r="AC269" s="13"/>
       <c r="AD269" s="13"/>
@@ -19261,7 +19271,7 @@
       <c r="X270" s="13"/>
       <c r="Y270" s="13"/>
       <c r="Z270" s="13"/>
-      <c r="AA270" s="13"/>
+      <c r="AA270" s="34"/>
       <c r="AB270" s="13"/>
       <c r="AC270" s="13"/>
       <c r="AD270" s="13"/>
@@ -19295,7 +19305,7 @@
       <c r="X271" s="13"/>
       <c r="Y271" s="13"/>
       <c r="Z271" s="13"/>
-      <c r="AA271" s="13"/>
+      <c r="AA271" s="34"/>
       <c r="AB271" s="13"/>
       <c r="AC271" s="13"/>
       <c r="AD271" s="13"/>
@@ -19329,7 +19339,7 @@
       <c r="X272" s="13"/>
       <c r="Y272" s="13"/>
       <c r="Z272" s="13"/>
-      <c r="AA272" s="13"/>
+      <c r="AA272" s="34"/>
       <c r="AB272" s="13"/>
       <c r="AC272" s="13"/>
       <c r="AD272" s="13"/>
@@ -19363,7 +19373,7 @@
       <c r="X273" s="13"/>
       <c r="Y273" s="13"/>
       <c r="Z273" s="13"/>
-      <c r="AA273" s="13"/>
+      <c r="AA273" s="34"/>
       <c r="AB273" s="13"/>
       <c r="AC273" s="13"/>
       <c r="AD273" s="13"/>
@@ -19397,7 +19407,7 @@
       <c r="X274" s="13"/>
       <c r="Y274" s="13"/>
       <c r="Z274" s="13"/>
-      <c r="AA274" s="13"/>
+      <c r="AA274" s="34"/>
       <c r="AB274" s="13"/>
       <c r="AC274" s="13"/>
       <c r="AD274" s="13"/>
@@ -19431,7 +19441,7 @@
       <c r="X275" s="13"/>
       <c r="Y275" s="13"/>
       <c r="Z275" s="13"/>
-      <c r="AA275" s="13"/>
+      <c r="AA275" s="34"/>
       <c r="AB275" s="13"/>
       <c r="AC275" s="13"/>
       <c r="AD275" s="13"/>
@@ -19465,7 +19475,7 @@
       <c r="X276" s="13"/>
       <c r="Y276" s="13"/>
       <c r="Z276" s="13"/>
-      <c r="AA276" s="13"/>
+      <c r="AA276" s="34"/>
       <c r="AB276" s="13"/>
       <c r="AC276" s="13"/>
       <c r="AD276" s="13"/>
@@ -19499,7 +19509,7 @@
       <c r="X277" s="13"/>
       <c r="Y277" s="13"/>
       <c r="Z277" s="13"/>
-      <c r="AA277" s="13"/>
+      <c r="AA277" s="34"/>
       <c r="AB277" s="13"/>
       <c r="AC277" s="13"/>
       <c r="AD277" s="13"/>
@@ -19533,7 +19543,7 @@
       <c r="X278" s="13"/>
       <c r="Y278" s="13"/>
       <c r="Z278" s="13"/>
-      <c r="AA278" s="13"/>
+      <c r="AA278" s="34"/>
       <c r="AB278" s="13"/>
       <c r="AC278" s="13"/>
       <c r="AD278" s="13"/>
@@ -19567,7 +19577,7 @@
       <c r="X279" s="13"/>
       <c r="Y279" s="13"/>
       <c r="Z279" s="13"/>
-      <c r="AA279" s="13"/>
+      <c r="AA279" s="34"/>
       <c r="AB279" s="13"/>
       <c r="AC279" s="13"/>
       <c r="AD279" s="13"/>
@@ -19601,7 +19611,7 @@
       <c r="X280" s="13"/>
       <c r="Y280" s="13"/>
       <c r="Z280" s="13"/>
-      <c r="AA280" s="13"/>
+      <c r="AA280" s="34"/>
       <c r="AB280" s="13"/>
       <c r="AC280" s="13"/>
       <c r="AD280" s="13"/>
@@ -19635,7 +19645,7 @@
       <c r="X281" s="13"/>
       <c r="Y281" s="13"/>
       <c r="Z281" s="13"/>
-      <c r="AA281" s="13"/>
+      <c r="AA281" s="34"/>
       <c r="AB281" s="13"/>
       <c r="AC281" s="13"/>
       <c r="AD281" s="13"/>
@@ -19669,7 +19679,7 @@
       <c r="X282" s="13"/>
       <c r="Y282" s="13"/>
       <c r="Z282" s="13"/>
-      <c r="AA282" s="13"/>
+      <c r="AA282" s="34"/>
       <c r="AB282" s="13"/>
       <c r="AC282" s="13"/>
       <c r="AD282" s="13"/>
@@ -19703,7 +19713,7 @@
       <c r="X283" s="13"/>
       <c r="Y283" s="13"/>
       <c r="Z283" s="13"/>
-      <c r="AA283" s="13"/>
+      <c r="AA283" s="34"/>
       <c r="AB283" s="13"/>
       <c r="AC283" s="13"/>
       <c r="AD283" s="13"/>
@@ -19737,7 +19747,7 @@
       <c r="X284" s="13"/>
       <c r="Y284" s="13"/>
       <c r="Z284" s="13"/>
-      <c r="AA284" s="13"/>
+      <c r="AA284" s="34"/>
       <c r="AB284" s="13"/>
       <c r="AC284" s="13"/>
       <c r="AD284" s="13"/>
@@ -19771,7 +19781,7 @@
       <c r="X285" s="13"/>
       <c r="Y285" s="13"/>
       <c r="Z285" s="13"/>
-      <c r="AA285" s="13"/>
+      <c r="AA285" s="34"/>
       <c r="AB285" s="13"/>
       <c r="AC285" s="13"/>
       <c r="AD285" s="13"/>
@@ -19805,7 +19815,7 @@
       <c r="X286" s="13"/>
       <c r="Y286" s="13"/>
       <c r="Z286" s="13"/>
-      <c r="AA286" s="13"/>
+      <c r="AA286" s="34"/>
       <c r="AB286" s="13"/>
       <c r="AC286" s="13"/>
       <c r="AD286" s="13"/>
@@ -19839,7 +19849,7 @@
       <c r="X287" s="13"/>
       <c r="Y287" s="13"/>
       <c r="Z287" s="13"/>
-      <c r="AA287" s="13"/>
+      <c r="AA287" s="34"/>
       <c r="AB287" s="13"/>
       <c r="AC287" s="13"/>
       <c r="AD287" s="13"/>
@@ -19873,7 +19883,7 @@
       <c r="X288" s="13"/>
       <c r="Y288" s="13"/>
       <c r="Z288" s="13"/>
-      <c r="AA288" s="13"/>
+      <c r="AA288" s="34"/>
       <c r="AB288" s="13"/>
       <c r="AC288" s="13"/>
       <c r="AD288" s="13"/>
@@ -19907,7 +19917,7 @@
       <c r="X289" s="13"/>
       <c r="Y289" s="13"/>
       <c r="Z289" s="13"/>
-      <c r="AA289" s="13"/>
+      <c r="AA289" s="34"/>
       <c r="AB289" s="13"/>
       <c r="AC289" s="13"/>
       <c r="AD289" s="13"/>
@@ -19941,7 +19951,7 @@
       <c r="X290" s="13"/>
       <c r="Y290" s="13"/>
       <c r="Z290" s="13"/>
-      <c r="AA290" s="13"/>
+      <c r="AA290" s="34"/>
       <c r="AB290" s="13"/>
       <c r="AC290" s="13"/>
       <c r="AD290" s="13"/>
@@ -19975,7 +19985,7 @@
       <c r="X291" s="13"/>
       <c r="Y291" s="13"/>
       <c r="Z291" s="13"/>
-      <c r="AA291" s="13"/>
+      <c r="AA291" s="34"/>
       <c r="AB291" s="13"/>
       <c r="AC291" s="13"/>
       <c r="AD291" s="13"/>
@@ -20009,7 +20019,7 @@
       <c r="X292" s="13"/>
       <c r="Y292" s="13"/>
       <c r="Z292" s="13"/>
-      <c r="AA292" s="13"/>
+      <c r="AA292" s="34"/>
       <c r="AB292" s="13"/>
       <c r="AC292" s="13"/>
       <c r="AD292" s="13"/>
@@ -20043,7 +20053,7 @@
       <c r="X293" s="13"/>
       <c r="Y293" s="13"/>
       <c r="Z293" s="13"/>
-      <c r="AA293" s="13"/>
+      <c r="AA293" s="34"/>
       <c r="AB293" s="13"/>
       <c r="AC293" s="13"/>
       <c r="AD293" s="13"/>
@@ -20077,7 +20087,7 @@
       <c r="X294" s="13"/>
       <c r="Y294" s="13"/>
       <c r="Z294" s="13"/>
-      <c r="AA294" s="13"/>
+      <c r="AA294" s="34"/>
       <c r="AB294" s="13"/>
       <c r="AC294" s="13"/>
       <c r="AD294" s="13"/>
@@ -20111,7 +20121,7 @@
       <c r="X295" s="13"/>
       <c r="Y295" s="13"/>
       <c r="Z295" s="13"/>
-      <c r="AA295" s="13"/>
+      <c r="AA295" s="34"/>
       <c r="AB295" s="13"/>
       <c r="AC295" s="13"/>
       <c r="AD295" s="13"/>
@@ -20145,7 +20155,7 @@
       <c r="X296" s="13"/>
       <c r="Y296" s="13"/>
       <c r="Z296" s="13"/>
-      <c r="AA296" s="13"/>
+      <c r="AA296" s="34"/>
       <c r="AB296" s="13"/>
       <c r="AC296" s="13"/>
       <c r="AD296" s="13"/>
@@ -20179,7 +20189,7 @@
       <c r="X297" s="13"/>
       <c r="Y297" s="13"/>
       <c r="Z297" s="13"/>
-      <c r="AA297" s="13"/>
+      <c r="AA297" s="34"/>
       <c r="AB297" s="13"/>
       <c r="AC297" s="13"/>
       <c r="AD297" s="13"/>
@@ -20213,7 +20223,7 @@
       <c r="X298" s="13"/>
       <c r="Y298" s="13"/>
       <c r="Z298" s="13"/>
-      <c r="AA298" s="13"/>
+      <c r="AA298" s="34"/>
       <c r="AB298" s="13"/>
       <c r="AC298" s="13"/>
       <c r="AD298" s="13"/>
@@ -20247,7 +20257,7 @@
       <c r="X299" s="13"/>
       <c r="Y299" s="13"/>
       <c r="Z299" s="13"/>
-      <c r="AA299" s="13"/>
+      <c r="AA299" s="34"/>
       <c r="AB299" s="13"/>
       <c r="AC299" s="13"/>
       <c r="AD299" s="13"/>
@@ -20281,7 +20291,7 @@
       <c r="X300" s="13"/>
       <c r="Y300" s="13"/>
       <c r="Z300" s="13"/>
-      <c r="AA300" s="13"/>
+      <c r="AA300" s="34"/>
       <c r="AB300" s="13"/>
       <c r="AC300" s="13"/>
       <c r="AD300" s="13"/>
@@ -20315,7 +20325,7 @@
       <c r="X301" s="13"/>
       <c r="Y301" s="13"/>
       <c r="Z301" s="13"/>
-      <c r="AA301" s="13"/>
+      <c r="AA301" s="34"/>
       <c r="AB301" s="13"/>
       <c r="AC301" s="13"/>
       <c r="AD301" s="13"/>
@@ -20349,7 +20359,7 @@
       <c r="X302" s="13"/>
       <c r="Y302" s="13"/>
       <c r="Z302" s="13"/>
-      <c r="AA302" s="13"/>
+      <c r="AA302" s="34"/>
       <c r="AB302" s="13"/>
       <c r="AC302" s="13"/>
       <c r="AD302" s="13"/>
@@ -20383,7 +20393,7 @@
       <c r="X303" s="13"/>
       <c r="Y303" s="13"/>
       <c r="Z303" s="13"/>
-      <c r="AA303" s="13"/>
+      <c r="AA303" s="34"/>
       <c r="AB303" s="13"/>
       <c r="AC303" s="13"/>
       <c r="AD303" s="13"/>
@@ -20417,7 +20427,7 @@
       <c r="X304" s="13"/>
       <c r="Y304" s="13"/>
       <c r="Z304" s="13"/>
-      <c r="AA304" s="13"/>
+      <c r="AA304" s="34"/>
       <c r="AB304" s="13"/>
       <c r="AC304" s="13"/>
       <c r="AD304" s="13"/>
@@ -20451,7 +20461,7 @@
       <c r="X305" s="13"/>
       <c r="Y305" s="13"/>
       <c r="Z305" s="13"/>
-      <c r="AA305" s="13"/>
+      <c r="AA305" s="34"/>
       <c r="AB305" s="13"/>
       <c r="AC305" s="13"/>
       <c r="AD305" s="13"/>
@@ -20485,7 +20495,7 @@
       <c r="X306" s="13"/>
       <c r="Y306" s="13"/>
       <c r="Z306" s="13"/>
-      <c r="AA306" s="13"/>
+      <c r="AA306" s="34"/>
       <c r="AB306" s="13"/>
       <c r="AC306" s="13"/>
       <c r="AD306" s="13"/>
@@ -20519,7 +20529,7 @@
       <c r="X307" s="13"/>
       <c r="Y307" s="13"/>
       <c r="Z307" s="13"/>
-      <c r="AA307" s="13"/>
+      <c r="AA307" s="34"/>
       <c r="AB307" s="13"/>
       <c r="AC307" s="13"/>
       <c r="AD307" s="13"/>
@@ -20553,7 +20563,7 @@
       <c r="X308" s="13"/>
       <c r="Y308" s="13"/>
       <c r="Z308" s="13"/>
-      <c r="AA308" s="13"/>
+      <c r="AA308" s="34"/>
       <c r="AB308" s="13"/>
       <c r="AC308" s="13"/>
       <c r="AD308" s="13"/>
@@ -20587,7 +20597,7 @@
       <c r="X309" s="13"/>
       <c r="Y309" s="13"/>
       <c r="Z309" s="13"/>
-      <c r="AA309" s="13"/>
+      <c r="AA309" s="34"/>
       <c r="AB309" s="13"/>
       <c r="AC309" s="13"/>
       <c r="AD309" s="13"/>
@@ -20621,7 +20631,7 @@
       <c r="X310" s="13"/>
       <c r="Y310" s="13"/>
       <c r="Z310" s="13"/>
-      <c r="AA310" s="13"/>
+      <c r="AA310" s="34"/>
       <c r="AB310" s="13"/>
       <c r="AC310" s="13"/>
       <c r="AD310" s="13"/>
@@ -20655,7 +20665,7 @@
       <c r="X311" s="13"/>
       <c r="Y311" s="13"/>
       <c r="Z311" s="13"/>
-      <c r="AA311" s="13"/>
+      <c r="AA311" s="34"/>
       <c r="AB311" s="13"/>
       <c r="AC311" s="13"/>
       <c r="AD311" s="13"/>
@@ -20689,7 +20699,7 @@
       <c r="X312" s="13"/>
       <c r="Y312" s="13"/>
       <c r="Z312" s="13"/>
-      <c r="AA312" s="13"/>
+      <c r="AA312" s="34"/>
       <c r="AB312" s="13"/>
       <c r="AC312" s="13"/>
       <c r="AD312" s="13"/>
@@ -20723,7 +20733,7 @@
       <c r="X313" s="13"/>
       <c r="Y313" s="13"/>
       <c r="Z313" s="13"/>
-      <c r="AA313" s="13"/>
+      <c r="AA313" s="34"/>
       <c r="AB313" s="13"/>
       <c r="AC313" s="13"/>
       <c r="AD313" s="13"/>
@@ -20757,7 +20767,7 @@
       <c r="X314" s="13"/>
       <c r="Y314" s="13"/>
       <c r="Z314" s="13"/>
-      <c r="AA314" s="13"/>
+      <c r="AA314" s="34"/>
       <c r="AB314" s="13"/>
       <c r="AC314" s="13"/>
       <c r="AD314" s="13"/>
@@ -20791,7 +20801,7 @@
       <c r="X315" s="13"/>
       <c r="Y315" s="13"/>
       <c r="Z315" s="13"/>
-      <c r="AA315" s="13"/>
+      <c r="AA315" s="34"/>
       <c r="AB315" s="13"/>
       <c r="AC315" s="13"/>
       <c r="AD315" s="13"/>
@@ -20825,7 +20835,7 @@
       <c r="X316" s="13"/>
       <c r="Y316" s="13"/>
       <c r="Z316" s="13"/>
-      <c r="AA316" s="13"/>
+      <c r="AA316" s="34"/>
       <c r="AB316" s="13"/>
       <c r="AC316" s="13"/>
       <c r="AD316" s="13"/>
@@ -20859,7 +20869,7 @@
       <c r="X317" s="13"/>
       <c r="Y317" s="13"/>
       <c r="Z317" s="13"/>
-      <c r="AA317" s="13"/>
+      <c r="AA317" s="34"/>
       <c r="AB317" s="13"/>
       <c r="AC317" s="13"/>
       <c r="AD317" s="13"/>
@@ -20893,7 +20903,7 @@
       <c r="X318" s="13"/>
       <c r="Y318" s="13"/>
       <c r="Z318" s="13"/>
-      <c r="AA318" s="13"/>
+      <c r="AA318" s="34"/>
       <c r="AB318" s="13"/>
       <c r="AC318" s="13"/>
       <c r="AD318" s="13"/>
@@ -20927,7 +20937,7 @@
       <c r="X319" s="13"/>
       <c r="Y319" s="13"/>
       <c r="Z319" s="13"/>
-      <c r="AA319" s="13"/>
+      <c r="AA319" s="34"/>
       <c r="AB319" s="13"/>
       <c r="AC319" s="13"/>
       <c r="AD319" s="13"/>
@@ -20961,7 +20971,7 @@
       <c r="X320" s="13"/>
       <c r="Y320" s="13"/>
       <c r="Z320" s="13"/>
-      <c r="AA320" s="13"/>
+      <c r="AA320" s="34"/>
       <c r="AB320" s="13"/>
       <c r="AC320" s="13"/>
       <c r="AD320" s="13"/>
@@ -20995,7 +21005,7 @@
       <c r="X321" s="13"/>
       <c r="Y321" s="13"/>
       <c r="Z321" s="13"/>
-      <c r="AA321" s="13"/>
+      <c r="AA321" s="34"/>
       <c r="AB321" s="13"/>
       <c r="AC321" s="13"/>
       <c r="AD321" s="13"/>
@@ -21029,7 +21039,7 @@
       <c r="X322" s="13"/>
       <c r="Y322" s="13"/>
       <c r="Z322" s="13"/>
-      <c r="AA322" s="13"/>
+      <c r="AA322" s="34"/>
       <c r="AB322" s="13"/>
       <c r="AC322" s="13"/>
       <c r="AD322" s="13"/>
@@ -21063,7 +21073,7 @@
       <c r="X323" s="13"/>
       <c r="Y323" s="13"/>
       <c r="Z323" s="13"/>
-      <c r="AA323" s="13"/>
+      <c r="AA323" s="34"/>
       <c r="AB323" s="13"/>
       <c r="AC323" s="13"/>
       <c r="AD323" s="13"/>
@@ -21097,7 +21107,7 @@
       <c r="X324" s="13"/>
       <c r="Y324" s="13"/>
       <c r="Z324" s="13"/>
-      <c r="AA324" s="13"/>
+      <c r="AA324" s="34"/>
       <c r="AB324" s="13"/>
       <c r="AC324" s="13"/>
       <c r="AD324" s="13"/>
@@ -21131,7 +21141,7 @@
       <c r="X325" s="13"/>
       <c r="Y325" s="13"/>
       <c r="Z325" s="13"/>
-      <c r="AA325" s="13"/>
+      <c r="AA325" s="34"/>
       <c r="AB325" s="13"/>
       <c r="AC325" s="13"/>
       <c r="AD325" s="13"/>
@@ -21165,7 +21175,7 @@
       <c r="X326" s="13"/>
       <c r="Y326" s="13"/>
       <c r="Z326" s="13"/>
-      <c r="AA326" s="13"/>
+      <c r="AA326" s="34"/>
       <c r="AB326" s="13"/>
       <c r="AC326" s="13"/>
       <c r="AD326" s="13"/>
@@ -21199,7 +21209,7 @@
       <c r="X327" s="13"/>
       <c r="Y327" s="13"/>
       <c r="Z327" s="13"/>
-      <c r="AA327" s="13"/>
+      <c r="AA327" s="34"/>
       <c r="AB327" s="13"/>
       <c r="AC327" s="13"/>
       <c r="AD327" s="13"/>
@@ -21233,7 +21243,7 @@
       <c r="X328" s="13"/>
       <c r="Y328" s="13"/>
       <c r="Z328" s="13"/>
-      <c r="AA328" s="13"/>
+      <c r="AA328" s="34"/>
       <c r="AB328" s="13"/>
       <c r="AC328" s="13"/>
       <c r="AD328" s="13"/>
@@ -21267,7 +21277,7 @@
       <c r="X329" s="13"/>
       <c r="Y329" s="13"/>
       <c r="Z329" s="13"/>
-      <c r="AA329" s="13"/>
+      <c r="AA329" s="34"/>
       <c r="AB329" s="13"/>
       <c r="AC329" s="13"/>
       <c r="AD329" s="13"/>
@@ -21301,7 +21311,7 @@
       <c r="X330" s="13"/>
       <c r="Y330" s="13"/>
       <c r="Z330" s="13"/>
-      <c r="AA330" s="13"/>
+      <c r="AA330" s="34"/>
       <c r="AB330" s="13"/>
       <c r="AC330" s="13"/>
       <c r="AD330" s="13"/>
@@ -21335,7 +21345,7 @@
       <c r="X331" s="13"/>
       <c r="Y331" s="13"/>
       <c r="Z331" s="13"/>
-      <c r="AA331" s="13"/>
+      <c r="AA331" s="34"/>
       <c r="AB331" s="13"/>
       <c r="AC331" s="13"/>
       <c r="AD331" s="13"/>
@@ -21369,7 +21379,7 @@
       <c r="X332" s="13"/>
       <c r="Y332" s="13"/>
       <c r="Z332" s="13"/>
-      <c r="AA332" s="13"/>
+      <c r="AA332" s="34"/>
       <c r="AB332" s="13"/>
       <c r="AC332" s="13"/>
       <c r="AD332" s="13"/>
@@ -21403,7 +21413,7 @@
       <c r="X333" s="13"/>
       <c r="Y333" s="13"/>
       <c r="Z333" s="13"/>
-      <c r="AA333" s="13"/>
+      <c r="AA333" s="34"/>
       <c r="AB333" s="13"/>
       <c r="AC333" s="13"/>
       <c r="AD333" s="13"/>
@@ -21437,7 +21447,7 @@
       <c r="X334" s="13"/>
       <c r="Y334" s="13"/>
       <c r="Z334" s="13"/>
-      <c r="AA334" s="13"/>
+      <c r="AA334" s="34"/>
       <c r="AB334" s="13"/>
       <c r="AC334" s="13"/>
       <c r="AD334" s="13"/>
@@ -21471,7 +21481,7 @@
       <c r="X335" s="13"/>
       <c r="Y335" s="13"/>
       <c r="Z335" s="13"/>
-      <c r="AA335" s="13"/>
+      <c r="AA335" s="34"/>
       <c r="AB335" s="13"/>
       <c r="AC335" s="13"/>
       <c r="AD335" s="13"/>
@@ -21505,7 +21515,7 @@
       <c r="X336" s="13"/>
       <c r="Y336" s="13"/>
       <c r="Z336" s="13"/>
-      <c r="AA336" s="13"/>
+      <c r="AA336" s="34"/>
       <c r="AB336" s="13"/>
       <c r="AC336" s="13"/>
       <c r="AD336" s="13"/>
@@ -21539,7 +21549,7 @@
       <c r="X337" s="13"/>
       <c r="Y337" s="13"/>
       <c r="Z337" s="13"/>
-      <c r="AA337" s="13"/>
+      <c r="AA337" s="34"/>
       <c r="AB337" s="13"/>
       <c r="AC337" s="13"/>
       <c r="AD337" s="13"/>
@@ -21573,7 +21583,7 @@
       <c r="X338" s="13"/>
       <c r="Y338" s="13"/>
       <c r="Z338" s="13"/>
-      <c r="AA338" s="13"/>
+      <c r="AA338" s="34"/>
       <c r="AB338" s="13"/>
       <c r="AC338" s="13"/>
       <c r="AD338" s="13"/>
@@ -21607,7 +21617,7 @@
       <c r="X339" s="13"/>
       <c r="Y339" s="13"/>
       <c r="Z339" s="13"/>
-      <c r="AA339" s="13"/>
+      <c r="AA339" s="34"/>
       <c r="AB339" s="13"/>
       <c r="AC339" s="13"/>
       <c r="AD339" s="13"/>
@@ -21641,7 +21651,7 @@
       <c r="X340" s="13"/>
       <c r="Y340" s="13"/>
       <c r="Z340" s="13"/>
-      <c r="AA340" s="13"/>
+      <c r="AA340" s="34"/>
       <c r="AB340" s="13"/>
       <c r="AC340" s="13"/>
       <c r="AD340" s="13"/>
@@ -21675,7 +21685,7 @@
       <c r="X341" s="13"/>
       <c r="Y341" s="13"/>
       <c r="Z341" s="13"/>
-      <c r="AA341" s="13"/>
+      <c r="AA341" s="34"/>
       <c r="AB341" s="13"/>
       <c r="AC341" s="13"/>
       <c r="AD341" s="13"/>
@@ -21709,7 +21719,7 @@
       <c r="X342" s="13"/>
       <c r="Y342" s="13"/>
       <c r="Z342" s="13"/>
-      <c r="AA342" s="13"/>
+      <c r="AA342" s="34"/>
       <c r="AB342" s="13"/>
       <c r="AC342" s="13"/>
       <c r="AD342" s="13"/>
@@ -21743,7 +21753,7 @@
       <c r="X343" s="13"/>
       <c r="Y343" s="13"/>
       <c r="Z343" s="13"/>
-      <c r="AA343" s="13"/>
+      <c r="AA343" s="34"/>
       <c r="AB343" s="13"/>
       <c r="AC343" s="13"/>
       <c r="AD343" s="13"/>
@@ -21777,7 +21787,7 @@
       <c r="X344" s="13"/>
       <c r="Y344" s="13"/>
       <c r="Z344" s="13"/>
-      <c r="AA344" s="13"/>
+      <c r="AA344" s="34"/>
       <c r="AB344" s="13"/>
       <c r="AC344" s="13"/>
       <c r="AD344" s="13"/>
@@ -21811,7 +21821,7 @@
       <c r="X345" s="13"/>
       <c r="Y345" s="13"/>
       <c r="Z345" s="13"/>
-      <c r="AA345" s="13"/>
+      <c r="AA345" s="34"/>
       <c r="AB345" s="13"/>
       <c r="AC345" s="13"/>
       <c r="AD345" s="13"/>
@@ -21845,7 +21855,7 @@
       <c r="X346" s="13"/>
       <c r="Y346" s="13"/>
       <c r="Z346" s="13"/>
-      <c r="AA346" s="13"/>
+      <c r="AA346" s="34"/>
       <c r="AB346" s="13"/>
       <c r="AC346" s="13"/>
       <c r="AD346" s="13"/>
@@ -21879,7 +21889,7 @@
       <c r="X347" s="13"/>
       <c r="Y347" s="13"/>
       <c r="Z347" s="13"/>
-      <c r="AA347" s="13"/>
+      <c r="AA347" s="34"/>
       <c r="AB347" s="13"/>
       <c r="AC347" s="13"/>
       <c r="AD347" s="13"/>
@@ -21913,7 +21923,7 @@
       <c r="X348" s="13"/>
       <c r="Y348" s="13"/>
       <c r="Z348" s="13"/>
-      <c r="AA348" s="13"/>
+      <c r="AA348" s="34"/>
       <c r="AB348" s="13"/>
       <c r="AC348" s="13"/>
       <c r="AD348" s="13"/>
@@ -21947,7 +21957,7 @@
       <c r="X349" s="13"/>
       <c r="Y349" s="13"/>
       <c r="Z349" s="13"/>
-      <c r="AA349" s="13"/>
+      <c r="AA349" s="34"/>
       <c r="AB349" s="13"/>
       <c r="AC349" s="13"/>
       <c r="AD349" s="13"/>
@@ -21981,7 +21991,7 @@
       <c r="X350" s="13"/>
       <c r="Y350" s="13"/>
       <c r="Z350" s="13"/>
-      <c r="AA350" s="13"/>
+      <c r="AA350" s="34"/>
       <c r="AB350" s="13"/>
       <c r="AC350" s="13"/>
       <c r="AD350" s="13"/>
@@ -22015,7 +22025,7 @@
       <c r="X351" s="13"/>
       <c r="Y351" s="13"/>
       <c r="Z351" s="13"/>
-      <c r="AA351" s="13"/>
+      <c r="AA351" s="34"/>
       <c r="AB351" s="13"/>
       <c r="AC351" s="13"/>
       <c r="AD351" s="13"/>
@@ -22049,7 +22059,7 @@
       <c r="X352" s="13"/>
       <c r="Y352" s="13"/>
       <c r="Z352" s="13"/>
-      <c r="AA352" s="13"/>
+      <c r="AA352" s="34"/>
       <c r="AB352" s="13"/>
       <c r="AC352" s="13"/>
       <c r="AD352" s="13"/>
@@ -22083,7 +22093,7 @@
       <c r="X353" s="13"/>
       <c r="Y353" s="13"/>
       <c r="Z353" s="13"/>
-      <c r="AA353" s="13"/>
+      <c r="AA353" s="34"/>
       <c r="AB353" s="13"/>
       <c r="AC353" s="13"/>
       <c r="AD353" s="13"/>
@@ -22117,7 +22127,7 @@
       <c r="X354" s="13"/>
       <c r="Y354" s="13"/>
       <c r="Z354" s="13"/>
-      <c r="AA354" s="13"/>
+      <c r="AA354" s="34"/>
       <c r="AB354" s="13"/>
       <c r="AC354" s="13"/>
       <c r="AD354" s="13"/>
@@ -22151,7 +22161,7 @@
       <c r="X355" s="13"/>
       <c r="Y355" s="13"/>
       <c r="Z355" s="13"/>
-      <c r="AA355" s="13"/>
+      <c r="AA355" s="34"/>
       <c r="AB355" s="13"/>
       <c r="AC355" s="13"/>
       <c r="AD355" s="13"/>
@@ -22185,7 +22195,7 @@
       <c r="X356" s="13"/>
       <c r="Y356" s="13"/>
       <c r="Z356" s="13"/>
-      <c r="AA356" s="13"/>
+      <c r="AA356" s="34"/>
       <c r="AB356" s="13"/>
       <c r="AC356" s="13"/>
       <c r="AD356" s="13"/>
@@ -22219,7 +22229,7 @@
       <c r="X357" s="13"/>
       <c r="Y357" s="13"/>
       <c r="Z357" s="13"/>
-      <c r="AA357" s="13"/>
+      <c r="AA357" s="34"/>
       <c r="AB357" s="13"/>
       <c r="AC357" s="13"/>
       <c r="AD357" s="13"/>
@@ -22253,7 +22263,7 @@
       <c r="X358" s="13"/>
       <c r="Y358" s="13"/>
       <c r="Z358" s="13"/>
-      <c r="AA358" s="13"/>
+      <c r="AA358" s="34"/>
       <c r="AB358" s="13"/>
       <c r="AC358" s="13"/>
       <c r="AD358" s="13"/>
@@ -22287,7 +22297,7 @@
       <c r="X359" s="13"/>
       <c r="Y359" s="13"/>
       <c r="Z359" s="13"/>
-      <c r="AA359" s="13"/>
+      <c r="AA359" s="34"/>
       <c r="AB359" s="13"/>
       <c r="AC359" s="13"/>
       <c r="AD359" s="13"/>
@@ -22321,7 +22331,7 @@
       <c r="X360" s="13"/>
       <c r="Y360" s="13"/>
       <c r="Z360" s="13"/>
-      <c r="AA360" s="13"/>
+      <c r="AA360" s="34"/>
       <c r="AB360" s="13"/>
       <c r="AC360" s="13"/>
       <c r="AD360" s="13"/>
@@ -22355,7 +22365,7 @@
       <c r="X361" s="13"/>
       <c r="Y361" s="13"/>
       <c r="Z361" s="13"/>
-      <c r="AA361" s="13"/>
+      <c r="AA361" s="34"/>
       <c r="AB361" s="13"/>
       <c r="AC361" s="13"/>
       <c r="AD361" s="13"/>
@@ -22389,7 +22399,7 @@
       <c r="X362" s="13"/>
       <c r="Y362" s="13"/>
       <c r="Z362" s="13"/>
-      <c r="AA362" s="13"/>
+      <c r="AA362" s="34"/>
       <c r="AB362" s="13"/>
       <c r="AC362" s="13"/>
       <c r="AD362" s="13"/>
@@ -22423,7 +22433,7 @@
       <c r="X363" s="13"/>
       <c r="Y363" s="13"/>
       <c r="Z363" s="13"/>
-      <c r="AA363" s="13"/>
+      <c r="AA363" s="34"/>
       <c r="AB363" s="13"/>
       <c r="AC363" s="13"/>
       <c r="AD363" s="13"/>
@@ -22457,7 +22467,7 @@
       <c r="X364" s="13"/>
       <c r="Y364" s="13"/>
       <c r="Z364" s="13"/>
-      <c r="AA364" s="13"/>
+      <c r="AA364" s="34"/>
       <c r="AB364" s="13"/>
       <c r="AC364" s="13"/>
       <c r="AD364" s="13"/>
@@ -22491,7 +22501,7 @@
       <c r="X365" s="13"/>
       <c r="Y365" s="13"/>
       <c r="Z365" s="13"/>
-      <c r="AA365" s="13"/>
+      <c r="AA365" s="34"/>
       <c r="AB365" s="13"/>
       <c r="AC365" s="13"/>
       <c r="AD365" s="13"/>
@@ -22525,7 +22535,7 @@
       <c r="X366" s="13"/>
       <c r="Y366" s="13"/>
       <c r="Z366" s="13"/>
-      <c r="AA366" s="13"/>
+      <c r="AA366" s="34"/>
       <c r="AB366" s="13"/>
       <c r="AC366" s="13"/>
       <c r="AD366" s="13"/>
@@ -22559,7 +22569,7 @@
       <c r="X367" s="13"/>
       <c r="Y367" s="13"/>
       <c r="Z367" s="13"/>
-      <c r="AA367" s="13"/>
+      <c r="AA367" s="34"/>
       <c r="AB367" s="13"/>
       <c r="AC367" s="13"/>
       <c r="AD367" s="13"/>
@@ -22593,7 +22603,7 @@
       <c r="X368" s="13"/>
       <c r="Y368" s="13"/>
       <c r="Z368" s="13"/>
-      <c r="AA368" s="13"/>
+      <c r="AA368" s="34"/>
       <c r="AB368" s="13"/>
       <c r="AC368" s="13"/>
       <c r="AD368" s="13"/>
@@ -22627,7 +22637,7 @@
       <c r="X369" s="13"/>
       <c r="Y369" s="13"/>
       <c r="Z369" s="13"/>
-      <c r="AA369" s="13"/>
+      <c r="AA369" s="34"/>
       <c r="AB369" s="13"/>
       <c r="AC369" s="13"/>
       <c r="AD369" s="13"/>
@@ -22661,7 +22671,7 @@
       <c r="X370" s="13"/>
       <c r="Y370" s="13"/>
       <c r="Z370" s="13"/>
-      <c r="AA370" s="13"/>
+      <c r="AA370" s="34"/>
       <c r="AB370" s="13"/>
       <c r="AC370" s="13"/>
       <c r="AD370" s="13"/>
@@ -22695,7 +22705,7 @@
       <c r="X371" s="13"/>
       <c r="Y371" s="13"/>
       <c r="Z371" s="13"/>
-      <c r="AA371" s="13"/>
+      <c r="AA371" s="34"/>
       <c r="AB371" s="13"/>
       <c r="AC371" s="13"/>
       <c r="AD371" s="13"/>
@@ -22729,7 +22739,7 @@
       <c r="X372" s="13"/>
       <c r="Y372" s="13"/>
       <c r="Z372" s="13"/>
-      <c r="AA372" s="13"/>
+      <c r="AA372" s="34"/>
       <c r="AB372" s="13"/>
       <c r="AC372" s="13"/>
       <c r="AD372" s="13"/>
@@ -22763,7 +22773,7 @@
       <c r="X373" s="13"/>
       <c r="Y373" s="13"/>
       <c r="Z373" s="13"/>
-      <c r="AA373" s="13"/>
+      <c r="AA373" s="34"/>
       <c r="AB373" s="13"/>
       <c r="AC373" s="13"/>
       <c r="AD373" s="13"/>
@@ -22797,7 +22807,7 @@
       <c r="X374" s="13"/>
       <c r="Y374" s="13"/>
       <c r="Z374" s="13"/>
-      <c r="AA374" s="13"/>
+      <c r="AA374" s="34"/>
       <c r="AB374" s="13"/>
       <c r="AC374" s="13"/>
       <c r="AD374" s="13"/>
@@ -22831,7 +22841,7 @@
       <c r="X375" s="13"/>
       <c r="Y375" s="13"/>
       <c r="Z375" s="13"/>
-      <c r="AA375" s="13"/>
+      <c r="AA375" s="34"/>
       <c r="AB375" s="13"/>
       <c r="AC375" s="13"/>
       <c r="AD375" s="13"/>
@@ -22865,7 +22875,7 @@
       <c r="X376" s="13"/>
       <c r="Y376" s="13"/>
       <c r="Z376" s="13"/>
-      <c r="AA376" s="13"/>
+      <c r="AA376" s="34"/>
       <c r="AB376" s="13"/>
       <c r="AC376" s="13"/>
       <c r="AD376" s="13"/>
@@ -22899,7 +22909,7 @@
       <c r="X377" s="13"/>
       <c r="Y377" s="13"/>
       <c r="Z377" s="13"/>
-      <c r="AA377" s="13"/>
+      <c r="AA377" s="34"/>
       <c r="AB377" s="13"/>
       <c r="AC377" s="13"/>
       <c r="AD377" s="13"/>
@@ -22933,7 +22943,7 @@
       <c r="X378" s="13"/>
       <c r="Y378" s="13"/>
       <c r="Z378" s="13"/>
-      <c r="AA378" s="13"/>
+      <c r="AA378" s="34"/>
       <c r="AB378" s="13"/>
       <c r="AC378" s="13"/>
       <c r="AD378" s="13"/>
@@ -22967,7 +22977,7 @@
       <c r="X379" s="13"/>
       <c r="Y379" s="13"/>
       <c r="Z379" s="13"/>
-      <c r="AA379" s="13"/>
+      <c r="AA379" s="34"/>
       <c r="AB379" s="13"/>
       <c r="AC379" s="13"/>
       <c r="AD379" s="13"/>
@@ -23001,7 +23011,7 @@
       <c r="X380" s="13"/>
       <c r="Y380" s="13"/>
       <c r="Z380" s="13"/>
-      <c r="AA380" s="13"/>
+      <c r="AA380" s="34"/>
       <c r="AB380" s="13"/>
       <c r="AC380" s="13"/>
       <c r="AD380" s="13"/>
@@ -23035,7 +23045,7 @@
       <c r="X381" s="13"/>
       <c r="Y381" s="13"/>
       <c r="Z381" s="13"/>
-      <c r="AA381" s="13"/>
+      <c r="AA381" s="34"/>
       <c r="AB381" s="13"/>
       <c r="AC381" s="13"/>
       <c r="AD381" s="13"/>
@@ -23069,7 +23079,7 @@
       <c r="X382" s="13"/>
       <c r="Y382" s="13"/>
       <c r="Z382" s="13"/>
-      <c r="AA382" s="13"/>
+      <c r="AA382" s="34"/>
       <c r="AB382" s="13"/>
       <c r="AC382" s="13"/>
       <c r="AD382" s="13"/>
@@ -23103,7 +23113,7 @@
       <c r="X383" s="13"/>
       <c r="Y383" s="13"/>
       <c r="Z383" s="13"/>
-      <c r="AA383" s="13"/>
+      <c r="AA383" s="34"/>
       <c r="AB383" s="13"/>
       <c r="AC383" s="13"/>
       <c r="AD383" s="13"/>
@@ -23137,7 +23147,7 @@
       <c r="X384" s="13"/>
       <c r="Y384" s="13"/>
       <c r="Z384" s="13"/>
-      <c r="AA384" s="13"/>
+      <c r="AA384" s="34"/>
       <c r="AB384" s="13"/>
       <c r="AC384" s="13"/>
       <c r="AD384" s="13"/>
@@ -23171,7 +23181,7 @@
       <c r="X385" s="13"/>
       <c r="Y385" s="13"/>
       <c r="Z385" s="13"/>
-      <c r="AA385" s="13"/>
+      <c r="AA385" s="34"/>
       <c r="AB385" s="13"/>
       <c r="AC385" s="13"/>
       <c r="AD385" s="13"/>
@@ -23205,7 +23215,7 @@
       <c r="X386" s="13"/>
       <c r="Y386" s="13"/>
       <c r="Z386" s="13"/>
-      <c r="AA386" s="13"/>
+      <c r="AA386" s="34"/>
       <c r="AB386" s="13"/>
       <c r="AC386" s="13"/>
       <c r="AD386" s="13"/>
@@ -23239,7 +23249,7 @@
       <c r="X387" s="13"/>
       <c r="Y387" s="13"/>
       <c r="Z387" s="13"/>
-      <c r="AA387" s="13"/>
+      <c r="AA387" s="34"/>
       <c r="AB387" s="13"/>
       <c r="AC387" s="13"/>
       <c r="AD387" s="13"/>
@@ -23273,7 +23283,7 @@
       <c r="X388" s="13"/>
       <c r="Y388" s="13"/>
       <c r="Z388" s="13"/>
-      <c r="AA388" s="13"/>
+      <c r="AA388" s="34"/>
       <c r="AB388" s="13"/>
       <c r="AC388" s="13"/>
       <c r="AD388" s="13"/>
@@ -23307,7 +23317,7 @@
       <c r="X389" s="13"/>
       <c r="Y389" s="13"/>
       <c r="Z389" s="13"/>
-      <c r="AA389" s="13"/>
+      <c r="AA389" s="34"/>
       <c r="AB389" s="13"/>
       <c r="AC389" s="13"/>
       <c r="AD389" s="13"/>
@@ -23341,7 +23351,7 @@
       <c r="X390" s="13"/>
       <c r="Y390" s="13"/>
       <c r="Z390" s="13"/>
-      <c r="AA390" s="13"/>
+      <c r="AA390" s="34"/>
       <c r="AB390" s="13"/>
       <c r="AC390" s="13"/>
       <c r="AD390" s="13"/>
@@ -23375,7 +23385,7 @@
       <c r="X391" s="13"/>
       <c r="Y391" s="13"/>
       <c r="Z391" s="13"/>
-      <c r="AA391" s="13"/>
+      <c r="AA391" s="34"/>
       <c r="AB391" s="13"/>
       <c r="AC391" s="13"/>
       <c r="AD391" s="13"/>
@@ -23409,7 +23419,7 @@
       <c r="X392" s="13"/>
       <c r="Y392" s="13"/>
       <c r="Z392" s="13"/>
-      <c r="AA392" s="13"/>
+      <c r="AA392" s="34"/>
       <c r="AB392" s="13"/>
       <c r="AC392" s="13"/>
       <c r="AD392" s="13"/>
@@ -23443,7 +23453,7 @@
       <c r="X393" s="13"/>
       <c r="Y393" s="13"/>
       <c r="Z393" s="13"/>
-      <c r="AA393" s="13"/>
+      <c r="AA393" s="34"/>
       <c r="AB393" s="13"/>
       <c r="AC393" s="13"/>
       <c r="AD393" s="13"/>
@@ -23477,7 +23487,7 @@
       <c r="X394" s="13"/>
       <c r="Y394" s="13"/>
       <c r="Z394" s="13"/>
-      <c r="AA394" s="13"/>
+      <c r="AA394" s="34"/>
       <c r="AB394" s="13"/>
       <c r="AC394" s="13"/>
       <c r="AD394" s="13"/>
@@ -23511,7 +23521,7 @@
       <c r="X395" s="13"/>
       <c r="Y395" s="13"/>
       <c r="Z395" s="13"/>
-      <c r="AA395" s="13"/>
+      <c r="AA395" s="34"/>
       <c r="AB395" s="13"/>
       <c r="AC395" s="13"/>
       <c r="AD395" s="13"/>
@@ -23545,7 +23555,7 @@
       <c r="X396" s="13"/>
       <c r="Y396" s="13"/>
       <c r="Z396" s="13"/>
-      <c r="AA396" s="13"/>
+      <c r="AA396" s="34"/>
       <c r="AB396" s="13"/>
       <c r="AC396" s="13"/>
       <c r="AD396" s="13"/>
@@ -23579,7 +23589,7 @@
       <c r="X397" s="13"/>
       <c r="Y397" s="13"/>
       <c r="Z397" s="13"/>
-      <c r="AA397" s="13"/>
+      <c r="AA397" s="34"/>
       <c r="AB397" s="13"/>
       <c r="AC397" s="13"/>
       <c r="AD397" s="13"/>
@@ -23613,7 +23623,7 @@
       <c r="X398" s="13"/>
       <c r="Y398" s="13"/>
       <c r="Z398" s="13"/>
-      <c r="AA398" s="13"/>
+      <c r="AA398" s="34"/>
       <c r="AB398" s="13"/>
       <c r="AC398" s="13"/>
       <c r="AD398" s="13"/>
@@ -23647,7 +23657,7 @@
       <c r="X399" s="13"/>
       <c r="Y399" s="13"/>
       <c r="Z399" s="13"/>
-      <c r="AA399" s="13"/>
+      <c r="AA399" s="34"/>
       <c r="AB399" s="13"/>
       <c r="AC399" s="13"/>
       <c r="AD399" s="13"/>
@@ -23681,7 +23691,7 @@
       <c r="X400" s="13"/>
       <c r="Y400" s="13"/>
       <c r="Z400" s="13"/>
-      <c r="AA400" s="13"/>
+      <c r="AA400" s="34"/>
       <c r="AB400" s="13"/>
       <c r="AC400" s="13"/>
       <c r="AD400" s="13"/>
@@ -23715,7 +23725,7 @@
       <c r="X401" s="13"/>
       <c r="Y401" s="13"/>
       <c r="Z401" s="13"/>
-      <c r="AA401" s="13"/>
+      <c r="AA401" s="34"/>
       <c r="AB401" s="13"/>
       <c r="AC401" s="13"/>
       <c r="AD401" s="13"/>
@@ -23749,7 +23759,7 @@
       <c r="X402" s="13"/>
       <c r="Y402" s="13"/>
       <c r="Z402" s="13"/>
-      <c r="AA402" s="13"/>
+      <c r="AA402" s="34"/>
       <c r="AB402" s="13"/>
       <c r="AC402" s="13"/>
       <c r="AD402" s="13"/>
@@ -23783,7 +23793,7 @@
       <c r="X403" s="13"/>
       <c r="Y403" s="13"/>
       <c r="Z403" s="13"/>
-      <c r="AA403" s="13"/>
+      <c r="AA403" s="34"/>
       <c r="AB403" s="13"/>
       <c r="AC403" s="13"/>
       <c r="AD403" s="13"/>
@@ -23817,7 +23827,7 @@
       <c r="X404" s="13"/>
       <c r="Y404" s="13"/>
       <c r="Z404" s="13"/>
-      <c r="AA404" s="13"/>
+      <c r="AA404" s="34"/>
       <c r="AB404" s="13"/>
       <c r="AC404" s="13"/>
       <c r="AD404" s="13"/>
@@ -23851,7 +23861,7 @@
       <c r="X405" s="13"/>
       <c r="Y405" s="13"/>
       <c r="Z405" s="13"/>
-      <c r="AA405" s="13"/>
+      <c r="AA405" s="34"/>
       <c r="AB405" s="13"/>
       <c r="AC405" s="13"/>
       <c r="AD405" s="13"/>
@@ -23885,7 +23895,7 @@
       <c r="X406" s="13"/>
       <c r="Y406" s="13"/>
       <c r="Z406" s="13"/>
-      <c r="AA406" s="13"/>
+      <c r="AA406" s="34"/>
       <c r="AB406" s="13"/>
       <c r="AC406" s="13"/>
       <c r="AD406" s="13"/>
@@ -23919,7 +23929,7 @@
       <c r="X407" s="13"/>
       <c r="Y407" s="13"/>
       <c r="Z407" s="13"/>
-      <c r="AA407" s="13"/>
+      <c r="AA407" s="34"/>
       <c r="AB407" s="13"/>
       <c r="AC407" s="13"/>
       <c r="AD407" s="13"/>
@@ -23953,7 +23963,7 @@
       <c r="X408" s="13"/>
       <c r="Y408" s="13"/>
       <c r="Z408" s="13"/>
-      <c r="AA408" s="13"/>
+      <c r="AA408" s="34"/>
       <c r="AB408" s="13"/>
       <c r="AC408" s="13"/>
       <c r="AD408" s="13"/>
@@ -23987,7 +23997,7 @@
       <c r="X409" s="13"/>
       <c r="Y409" s="13"/>
       <c r="Z409" s="13"/>
-      <c r="AA409" s="13"/>
+      <c r="AA409" s="34"/>
       <c r="AB409" s="13"/>
       <c r="AC409" s="13"/>
       <c r="AD409" s="13"/>
@@ -24021,7 +24031,7 @@
       <c r="X410" s="13"/>
       <c r="Y410" s="13"/>
       <c r="Z410" s="13"/>
-      <c r="AA410" s="13"/>
+      <c r="AA410" s="34"/>
       <c r="AB410" s="13"/>
       <c r="AC410" s="13"/>
       <c r="AD410" s="13"/>
@@ -24055,7 +24065,7 @@
       <c r="X411" s="13"/>
       <c r="Y411" s="13"/>
       <c r="Z411" s="13"/>
-      <c r="AA411" s="13"/>
+      <c r="AA411" s="34"/>
       <c r="AB411" s="13"/>
       <c r="AC411" s="13"/>
       <c r="AD411" s="13"/>
@@ -24089,7 +24099,7 @@
       <c r="X412" s="13"/>
       <c r="Y412" s="13"/>
       <c r="Z412" s="13"/>
-      <c r="AA412" s="13"/>
+      <c r="AA412" s="34"/>
       <c r="AB412" s="13"/>
       <c r="AC412" s="13"/>
       <c r="AD412" s="13"/>
@@ -24123,7 +24133,7 @@
       <c r="X413" s="13"/>
       <c r="Y413" s="13"/>
       <c r="Z413" s="13"/>
-      <c r="AA413" s="13"/>
+      <c r="AA413" s="34"/>
       <c r="AB413" s="13"/>
       <c r="AC413" s="13"/>
       <c r="AD413" s="13"/>
@@ -24157,7 +24167,7 @@
       <c r="X414" s="13"/>
       <c r="Y414" s="13"/>
       <c r="Z414" s="13"/>
-      <c r="AA414" s="13"/>
+      <c r="AA414" s="34"/>
       <c r="AB414" s="13"/>
       <c r="AC414" s="13"/>
       <c r="AD414" s="13"/>
@@ -24191,7 +24201,7 @@
       <c r="X415" s="13"/>
       <c r="Y415" s="13"/>
       <c r="Z415" s="13"/>
-      <c r="AA415" s="13"/>
+      <c r="AA415" s="34"/>
       <c r="AB415" s="13"/>
       <c r="AC415" s="13"/>
       <c r="AD415" s="13"/>
@@ -24225,7 +24235,7 @@
       <c r="X416" s="13"/>
       <c r="Y416" s="13"/>
       <c r="Z416" s="13"/>
-      <c r="AA416" s="13"/>
+      <c r="AA416" s="34"/>
       <c r="AB416" s="13"/>
       <c r="AC416" s="13"/>
       <c r="AD416" s="13"/>
@@ -24259,7 +24269,7 @@
       <c r="X417" s="13"/>
       <c r="Y417" s="13"/>
       <c r="Z417" s="13"/>
-      <c r="AA417" s="13"/>
+      <c r="AA417" s="34"/>
       <c r="AB417" s="13"/>
       <c r="AC417" s="13"/>
       <c r="AD417" s="13"/>
@@ -24293,7 +24303,7 @@
       <c r="X418" s="13"/>
       <c r="Y418" s="13"/>
       <c r="Z418" s="13"/>
-      <c r="AA418" s="13"/>
+      <c r="AA418" s="34"/>
       <c r="AB418" s="13"/>
       <c r="AC418" s="13"/>
       <c r="AD418" s="13"/>
@@ -24327,7 +24337,7 @@
       <c r="X419" s="13"/>
       <c r="Y419" s="13"/>
       <c r="Z419" s="13"/>
-      <c r="AA419" s="13"/>
+      <c r="AA419" s="34"/>
       <c r="AB419" s="13"/>
       <c r="AC419" s="13"/>
       <c r="AD419" s="13"/>
@@ -24361,7 +24371,7 @@
       <c r="X420" s="13"/>
       <c r="Y420" s="13"/>
       <c r="Z420" s="13"/>
-      <c r="AA420" s="13"/>
+      <c r="AA420" s="34"/>
       <c r="AB420" s="13"/>
       <c r="AC420" s="13"/>
       <c r="AD420" s="13"/>
@@ -24395,7 +24405,7 @@
       <c r="X421" s="13"/>
       <c r="Y421" s="13"/>
       <c r="Z421" s="13"/>
-      <c r="AA421" s="13"/>
+      <c r="AA421" s="34"/>
       <c r="AB421" s="13"/>
       <c r="AC421" s="13"/>
       <c r="AD421" s="13"/>
@@ -24429,7 +24439,7 @@
       <c r="X422" s="13"/>
       <c r="Y422" s="13"/>
       <c r="Z422" s="13"/>
-      <c r="AA422" s="13"/>
+      <c r="AA422" s="34"/>
       <c r="AB422" s="13"/>
       <c r="AC422" s="13"/>
       <c r="AD422" s="13"/>
@@ -24463,7 +24473,7 @@
       <c r="X423" s="13"/>
       <c r="Y423" s="13"/>
       <c r="Z423" s="13"/>
-      <c r="AA423" s="13"/>
+      <c r="AA423" s="34"/>
       <c r="AB423" s="13"/>
       <c r="AC423" s="13"/>
       <c r="AD423" s="13"/>
@@ -24497,7 +24507,7 @@
       <c r="X424" s="13"/>
       <c r="Y424" s="13"/>
       <c r="Z424" s="13"/>
-      <c r="AA424" s="13"/>
+      <c r="AA424" s="34"/>
       <c r="AB424" s="13"/>
       <c r="AC424" s="13"/>
       <c r="AD424" s="13"/>
@@ -24531,7 +24541,7 @@
       <c r="X425" s="13"/>
       <c r="Y425" s="13"/>
       <c r="Z425" s="13"/>
-      <c r="AA425" s="13"/>
+      <c r="AA425" s="34"/>
       <c r="AB425" s="13"/>
       <c r="AC425" s="13"/>
       <c r="AD425" s="13"/>
@@ -24565,7 +24575,7 @@
       <c r="X426" s="13"/>
       <c r="Y426" s="13"/>
       <c r="Z426" s="13"/>
-      <c r="AA426" s="13"/>
+      <c r="AA426" s="34"/>
       <c r="AB426" s="13"/>
       <c r="AC426" s="13"/>
       <c r="AD426" s="13"/>
@@ -24599,7 +24609,7 @@
       <c r="X427" s="13"/>
       <c r="Y427" s="13"/>
       <c r="Z427" s="13"/>
-      <c r="AA427" s="13"/>
+      <c r="AA427" s="34"/>
       <c r="AB427" s="13"/>
       <c r="AC427" s="13"/>
       <c r="AD427" s="13"/>
@@ -24633,7 +24643,7 @@
       <c r="X428" s="13"/>
       <c r="Y428" s="13"/>
       <c r="Z428" s="13"/>
-      <c r="AA428" s="13"/>
+      <c r="AA428" s="34"/>
       <c r="AB428" s="13"/>
       <c r="AC428" s="13"/>
       <c r="AD428" s="13"/>
@@ -24667,7 +24677,7 @@
       <c r="X429" s="13"/>
       <c r="Y429" s="13"/>
       <c r="Z429" s="13"/>
-      <c r="AA429" s="13"/>
+      <c r="AA429" s="34"/>
       <c r="AB429" s="13"/>
       <c r="AC429" s="13"/>
       <c r="AD429" s="13"/>
@@ -24701,7 +24711,7 @@
       <c r="X430" s="13"/>
       <c r="Y430" s="13"/>
       <c r="Z430" s="13"/>
-      <c r="AA430" s="13"/>
+      <c r="AA430" s="34"/>
       <c r="AB430" s="13"/>
       <c r="AC430" s="13"/>
       <c r="AD430" s="13"/>
@@ -24735,7 +24745,7 @@
       <c r="X431" s="13"/>
       <c r="Y431" s="13"/>
       <c r="Z431" s="13"/>
-      <c r="AA431" s="13"/>
+      <c r="AA431" s="34"/>
       <c r="AB431" s="13"/>
       <c r="AC431" s="13"/>
       <c r="AD431" s="13"/>
@@ -24769,7 +24779,7 @@
       <c r="X432" s="13"/>
       <c r="Y432" s="13"/>
       <c r="Z432" s="13"/>
-      <c r="AA432" s="13"/>
+      <c r="AA432" s="34"/>
       <c r="AB432" s="13"/>
       <c r="AC432" s="13"/>
       <c r="AD432" s="13"/>
@@ -24803,7 +24813,7 @@
       <c r="X433" s="13"/>
       <c r="Y433" s="13"/>
       <c r="Z433" s="13"/>
-      <c r="AA433" s="13"/>
+      <c r="AA433" s="34"/>
       <c r="AB433" s="13"/>
       <c r="AC433" s="13"/>
       <c r="AD433" s="13"/>
@@ -24837,7 +24847,7 @@
       <c r="X434" s="13"/>
       <c r="Y434" s="13"/>
       <c r="Z434" s="13"/>
-      <c r="AA434" s="13"/>
+      <c r="AA434" s="34"/>
       <c r="AB434" s="13"/>
       <c r="AC434" s="13"/>
       <c r="AD434" s="13"/>
@@ -24871,7 +24881,7 @@
       <c r="X435" s="13"/>
       <c r="Y435" s="13"/>
       <c r="Z435" s="13"/>
-      <c r="AA435" s="13"/>
+      <c r="AA435" s="34"/>
       <c r="AB435" s="13"/>
       <c r="AC435" s="13"/>
       <c r="AD435" s="13"/>
@@ -24905,7 +24915,7 @@
       <c r="X436" s="13"/>
       <c r="Y436" s="13"/>
       <c r="Z436" s="13"/>
-      <c r="AA436" s="13"/>
+      <c r="AA436" s="34"/>
       <c r="AB436" s="13"/>
       <c r="AC436" s="13"/>
       <c r="AD436" s="13"/>
@@ -24939,7 +24949,7 @@
       <c r="X437" s="13"/>
       <c r="Y437" s="13"/>
       <c r="Z437" s="13"/>
-      <c r="AA437" s="13"/>
+      <c r="AA437" s="34"/>
       <c r="AB437" s="13"/>
       <c r="AC437" s="13"/>
       <c r="AD437" s="13"/>
@@ -24973,7 +24983,7 @@
       <c r="X438" s="13"/>
       <c r="Y438" s="13"/>
       <c r="Z438" s="13"/>
-      <c r="AA438" s="13"/>
+      <c r="AA438" s="34"/>
       <c r="AB438" s="13"/>
       <c r="AC438" s="13"/>
       <c r="AD438" s="13"/>
@@ -25007,7 +25017,7 @@
       <c r="X439" s="13"/>
       <c r="Y439" s="13"/>
       <c r="Z439" s="13"/>
-      <c r="AA439" s="13"/>
+      <c r="AA439" s="34"/>
       <c r="AB439" s="13"/>
       <c r="AC439" s="13"/>
       <c r="AD439" s="13"/>
@@ -25041,7 +25051,7 @@
       <c r="X440" s="13"/>
       <c r="Y440" s="13"/>
       <c r="Z440" s="13"/>
-      <c r="AA440" s="13"/>
+      <c r="AA440" s="34"/>
       <c r="AB440" s="13"/>
       <c r="AC440" s="13"/>
       <c r="AD440" s="13"/>
@@ -25075,7 +25085,7 @@
       <c r="X441" s="13"/>
       <c r="Y441" s="13"/>
       <c r="Z441" s="13"/>
-      <c r="AA441" s="13"/>
+      <c r="AA441" s="34"/>
       <c r="AB441" s="13"/>
       <c r="AC441" s="13"/>
       <c r="AD441" s="13"/>
@@ -25109,7 +25119,7 @@
       <c r="X442" s="13"/>
       <c r="Y442" s="13"/>
       <c r="Z442" s="13"/>
-      <c r="AA442" s="13"/>
+      <c r="AA442" s="34"/>
       <c r="AB442" s="13"/>
       <c r="AC442" s="13"/>
       <c r="AD442" s="13"/>
@@ -25143,7 +25153,7 @@
       <c r="X443" s="13"/>
       <c r="Y443" s="13"/>
       <c r="Z443" s="13"/>
-      <c r="AA443" s="13"/>
+      <c r="AA443" s="34"/>
       <c r="AB443" s="13"/>
       <c r="AC443" s="13"/>
       <c r="AD443" s="13"/>
@@ -25177,7 +25187,7 @@
       <c r="X444" s="13"/>
       <c r="Y444" s="13"/>
       <c r="Z444" s="13"/>
-      <c r="AA444" s="13"/>
+      <c r="AA444" s="34"/>
       <c r="AB444" s="13"/>
       <c r="AC444" s="13"/>
       <c r="AD444" s="13"/>
@@ -25211,7 +25221,7 @@
       <c r="X445" s="13"/>
       <c r="Y445" s="13"/>
       <c r="Z445" s="13"/>
-      <c r="AA445" s="13"/>
+      <c r="AA445" s="34"/>
       <c r="AB445" s="13"/>
       <c r="AC445" s="13"/>
       <c r="AD445" s="13"/>
@@ -25245,7 +25255,7 @@
       <c r="X446" s="13"/>
       <c r="Y446" s="13"/>
       <c r="Z446" s="13"/>
-      <c r="AA446" s="13"/>
+      <c r="AA446" s="34"/>
       <c r="AB446" s="13"/>
       <c r="AC446" s="13"/>
       <c r="AD446" s="13"/>
@@ -25279,7 +25289,7 @@
       <c r="X447" s="13"/>
       <c r="Y447" s="13"/>
       <c r="Z447" s="13"/>
-      <c r="AA447" s="13"/>
+      <c r="AA447" s="34"/>
       <c r="AB447" s="13"/>
       <c r="AC447" s="13"/>
       <c r="AD447" s="13"/>
@@ -25313,7 +25323,7 @@
       <c r="X448" s="13"/>
       <c r="Y448" s="13"/>
       <c r="Z448" s="13"/>
-      <c r="AA448" s="13"/>
+      <c r="AA448" s="34"/>
       <c r="AB448" s="13"/>
       <c r="AC448" s="13"/>
       <c r="AD448" s="13"/>
@@ -25347,7 +25357,7 @@
       <c r="X449" s="13"/>
       <c r="Y449" s="13"/>
       <c r="Z449" s="13"/>
-      <c r="AA449" s="13"/>
+      <c r="AA449" s="34"/>
       <c r="AB449" s="13"/>
       <c r="AC449" s="13"/>
       <c r="AD449" s="13"/>
@@ -25381,7 +25391,7 @@
       <c r="X450" s="13"/>
       <c r="Y450" s="13"/>
       <c r="Z450" s="13"/>
-      <c r="AA450" s="13"/>
+      <c r="AA450" s="34"/>
       <c r="AB450" s="13"/>
       <c r="AC450" s="13"/>
       <c r="AD450" s="13"/>
@@ -25415,7 +25425,7 @@
       <c r="X451" s="13"/>
       <c r="Y451" s="13"/>
       <c r="Z451" s="13"/>
-      <c r="AA451" s="13"/>
+      <c r="AA451" s="34"/>
       <c r="AB451" s="13"/>
       <c r="AC451" s="13"/>
       <c r="AD451" s="13"/>
@@ -25449,7 +25459,7 @@
       <c r="X452" s="13"/>
       <c r="Y452" s="13"/>
       <c r="Z452" s="13"/>
-      <c r="AA452" s="13"/>
+      <c r="AA452" s="34"/>
       <c r="AB452" s="13"/>
       <c r="AC452" s="13"/>
       <c r="AD452" s="13"/>
@@ -25483,7 +25493,7 @@
       <c r="X453" s="13"/>
       <c r="Y453" s="13"/>
       <c r="Z453" s="13"/>
-      <c r="AA453" s="13"/>
+      <c r="AA453" s="34"/>
       <c r="AB453" s="13"/>
       <c r="AC453" s="13"/>
       <c r="AD453" s="13"/>
@@ -25517,7 +25527,7 @@
       <c r="X454" s="13"/>
       <c r="Y454" s="13"/>
       <c r="Z454" s="13"/>
-      <c r="AA454" s="13"/>
+      <c r="AA454" s="34"/>
       <c r="AB454" s="13"/>
       <c r="AC454" s="13"/>
       <c r="AD454" s="13"/>
@@ -25551,7 +25561,7 @@
       <c r="X455" s="13"/>
       <c r="Y455" s="13"/>
       <c r="Z455" s="13"/>
-      <c r="AA455" s="13"/>
+      <c r="AA455" s="34"/>
       <c r="AB455" s="13"/>
       <c r="AC455" s="13"/>
       <c r="AD455" s="13"/>
@@ -25585,7 +25595,7 @@
       <c r="X456" s="13"/>
       <c r="Y456" s="13"/>
       <c r="Z456" s="13"/>
-      <c r="AA456" s="13"/>
+      <c r="AA456" s="34"/>
       <c r="AB456" s="13"/>
       <c r="AC456" s="13"/>
       <c r="AD456" s="13"/>
@@ -25619,7 +25629,7 @@
       <c r="X457" s="13"/>
       <c r="Y457" s="13"/>
       <c r="Z457" s="13"/>
-      <c r="AA457" s="13"/>
+      <c r="AA457" s="34"/>
       <c r="AB457" s="13"/>
       <c r="AC457" s="13"/>
       <c r="AD457" s="13"/>
@@ -25653,7 +25663,7 @@
       <c r="X458" s="13"/>
       <c r="Y458" s="13"/>
       <c r="Z458" s="13"/>
-      <c r="AA458" s="13"/>
+      <c r="AA458" s="34"/>
       <c r="AB458" s="13"/>
       <c r="AC458" s="13"/>
       <c r="AD458" s="13"/>
@@ -25687,7 +25697,7 @@
       <c r="X459" s="13"/>
       <c r="Y459" s="13"/>
       <c r="Z459" s="13"/>
-      <c r="AA459" s="13"/>
+      <c r="AA459" s="34"/>
       <c r="AB459" s="13"/>
       <c r="AC459" s="13"/>
       <c r="AD459" s="13"/>
@@ -25721,7 +25731,7 @@
       <c r="X460" s="13"/>
       <c r="Y460" s="13"/>
       <c r="Z460" s="13"/>
-      <c r="AA460" s="13"/>
+      <c r="AA460" s="34"/>
       <c r="AB460" s="13"/>
       <c r="AC460" s="13"/>
       <c r="AD460" s="13"/>
@@ -25755,7 +25765,7 @@
       <c r="X461" s="13"/>
       <c r="Y461" s="13"/>
       <c r="Z461" s="13"/>
-      <c r="AA461" s="13"/>
+      <c r="AA461" s="34"/>
       <c r="AB461" s="13"/>
       <c r="AC461" s="13"/>
       <c r="AD461" s="13"/>
@@ -25789,7 +25799,7 @@
       <c r="X462" s="13"/>
       <c r="Y462" s="13"/>
       <c r="Z462" s="13"/>
-      <c r="AA462" s="13"/>
+      <c r="AA462" s="34"/>
       <c r="AB462" s="13"/>
       <c r="AC462" s="13"/>
       <c r="AD462" s="13"/>
@@ -25823,7 +25833,7 @@
       <c r="X463" s="13"/>
       <c r="Y463" s="13"/>
       <c r="Z463" s="13"/>
-      <c r="AA463" s="13"/>
+      <c r="AA463" s="34"/>
       <c r="AB463" s="13"/>
       <c r="AC463" s="13"/>
       <c r="AD463" s="13"/>
@@ -25857,7 +25867,7 @@
       <c r="X464" s="13"/>
       <c r="Y464" s="13"/>
       <c r="Z464" s="13"/>
-      <c r="AA464" s="13"/>
+      <c r="AA464" s="34"/>
       <c r="AB464" s="13"/>
       <c r="AC464" s="13"/>
       <c r="AD464" s="13"/>
@@ -25891,7 +25901,7 @@
       <c r="X465" s="13"/>
       <c r="Y465" s="13"/>
       <c r="Z465" s="13"/>
-      <c r="AA465" s="13"/>
+      <c r="AA465" s="34"/>
       <c r="AB465" s="13"/>
       <c r="AC465" s="13"/>
       <c r="AD465" s="13"/>
@@ -25925,7 +25935,7 @@
       <c r="X466" s="13"/>
       <c r="Y466" s="13"/>
       <c r="Z466" s="13"/>
-      <c r="AA466" s="13"/>
+      <c r="AA466" s="34"/>
       <c r="AB466" s="13"/>
       <c r="AC466" s="13"/>
       <c r="AD466" s="13"/>
@@ -25959,7 +25969,7 @@
       <c r="X467" s="13"/>
       <c r="Y467" s="13"/>
       <c r="Z467" s="13"/>
-      <c r="AA467" s="13"/>
+      <c r="AA467" s="34"/>
       <c r="AB467" s="13"/>
       <c r="AC467" s="13"/>
       <c r="AD467" s="13"/>
@@ -25993,7 +26003,7 @@
       <c r="X468" s="13"/>
       <c r="Y468" s="13"/>
       <c r="Z468" s="13"/>
-      <c r="AA468" s="13"/>
+      <c r="AA468" s="34"/>
       <c r="AB468" s="13"/>
       <c r="AC468" s="13"/>
       <c r="AD468" s="13"/>
@@ -26027,7 +26037,7 @@
       <c r="X469" s="13"/>
       <c r="Y469" s="13"/>
       <c r="Z469" s="13"/>
-      <c r="AA469" s="13"/>
+      <c r="AA469" s="34"/>
       <c r="AB469" s="13"/>
       <c r="AC469" s="13"/>
       <c r="AD469" s="13"/>
@@ -26061,7 +26071,7 @@
       <c r="X470" s="13"/>
       <c r="Y470" s="13"/>
       <c r="Z470" s="13"/>
-      <c r="AA470" s="13"/>
+      <c r="AA470" s="34"/>
       <c r="AB470" s="13"/>
       <c r="AC470" s="13"/>
       <c r="AD470" s="13"/>
@@ -26095,7 +26105,7 @@
       <c r="X471" s="13"/>
       <c r="Y471" s="13"/>
       <c r="Z471" s="13"/>
-      <c r="AA471" s="13"/>
+      <c r="AA471" s="34"/>
       <c r="AB471" s="13"/>
       <c r="AC471" s="13"/>
       <c r="AD471" s="13"/>
@@ -26129,7 +26139,7 @@
       <c r="X472" s="13"/>
       <c r="Y472" s="13"/>
       <c r="Z472" s="13"/>
-      <c r="AA472" s="13"/>
+      <c r="AA472" s="34"/>
       <c r="AB472" s="13"/>
       <c r="AC472" s="13"/>
       <c r="AD472" s="13"/>
@@ -26163,7 +26173,7 @@
       <c r="X473" s="13"/>
       <c r="Y473" s="13"/>
       <c r="Z473" s="13"/>
-      <c r="AA473" s="13"/>
+      <c r="AA473" s="34"/>
       <c r="AB473" s="13"/>
       <c r="AC473" s="13"/>
       <c r="AD473" s="13"/>
@@ -26197,7 +26207,7 @@
       <c r="X474" s="13"/>
       <c r="Y474" s="13"/>
       <c r="Z474" s="13"/>
-      <c r="AA474" s="13"/>
+      <c r="AA474" s="34"/>
       <c r="AB474" s="13"/>
       <c r="AC474" s="13"/>
       <c r="AD474" s="13"/>
@@ -26231,7 +26241,7 @@
       <c r="X475" s="13"/>
       <c r="Y475" s="13"/>
       <c r="Z475" s="13"/>
-      <c r="AA475" s="13"/>
+      <c r="AA475" s="34"/>
       <c r="AB475" s="13"/>
       <c r="AC475" s="13"/>
       <c r="AD475" s="13"/>
@@ -26265,7 +26275,7 @@
       <c r="X476" s="13"/>
       <c r="Y476" s="13"/>
       <c r="Z476" s="13"/>
-      <c r="AA476" s="13"/>
+      <c r="AA476" s="34"/>
       <c r="AB476" s="13"/>
       <c r="AC476" s="13"/>
       <c r="AD476" s="13"/>
@@ -26299,7 +26309,7 @@
       <c r="X477" s="13"/>
       <c r="Y477" s="13"/>
       <c r="Z477" s="13"/>
-      <c r="AA477" s="13"/>
+      <c r="AA477" s="34"/>
       <c r="AB477" s="13"/>
       <c r="AC477" s="13"/>
       <c r="AD477" s="13"/>
@@ -26333,7 +26343,7 @@
       <c r="X478" s="13"/>
       <c r="Y478" s="13"/>
       <c r="Z478" s="13"/>
-      <c r="AA478" s="13"/>
+      <c r="AA478" s="34"/>
       <c r="AB478" s="13"/>
       <c r="AC478" s="13"/>
       <c r="AD478" s="13"/>
@@ -26367,7 +26377,7 @@
       <c r="X479" s="13"/>
       <c r="Y479" s="13"/>
       <c r="Z479" s="13"/>
-      <c r="AA479" s="13"/>
+      <c r="AA479" s="34"/>
       <c r="AB479" s="13"/>
       <c r="AC479" s="13"/>
       <c r="AD479" s="13"/>
@@ -26401,7 +26411,7 @@
       <c r="X480" s="13"/>
       <c r="Y480" s="13"/>
       <c r="Z480" s="13"/>
-      <c r="AA480" s="13"/>
+      <c r="AA480" s="34"/>
       <c r="AB480" s="13"/>
       <c r="AC480" s="13"/>
       <c r="AD480" s="13"/>
@@ -26435,7 +26445,7 @@
       <c r="X481" s="13"/>
       <c r="Y481" s="13"/>
       <c r="Z481" s="13"/>
-      <c r="AA481" s="13"/>
+      <c r="AA481" s="34"/>
       <c r="AB481" s="13"/>
       <c r="AC481" s="13"/>
       <c r="AD481" s="13"/>
@@ -26469,7 +26479,7 @@
       <c r="X482" s="13"/>
       <c r="Y482" s="13"/>
       <c r="Z482" s="13"/>
-      <c r="AA482" s="13"/>
+      <c r="AA482" s="34"/>
       <c r="AB482" s="13"/>
       <c r="AC482" s="13"/>
       <c r="AD482" s="13"/>
@@ -26503,7 +26513,7 @@
       <c r="X483" s="13"/>
       <c r="Y483" s="13"/>
       <c r="Z483" s="13"/>
-      <c r="AA483" s="13"/>
+      <c r="AA483" s="34"/>
       <c r="AB483" s="13"/>
       <c r="AC483" s="13"/>
       <c r="AD483" s="13"/>
@@ -26537,7 +26547,7 @@
       <c r="X484" s="13"/>
       <c r="Y484" s="13"/>
       <c r="Z484" s="13"/>
-      <c r="AA484" s="13"/>
+      <c r="AA484" s="34"/>
       <c r="AB484" s="13"/>
       <c r="AC484" s="13"/>
       <c r="AD484" s="13"/>
@@ -26571,7 +26581,7 @@
       <c r="X485" s="13"/>
       <c r="Y485" s="13"/>
       <c r="Z485" s="13"/>
-      <c r="AA485" s="13"/>
+      <c r="AA485" s="34"/>
       <c r="AB485" s="13"/>
       <c r="AC485" s="13"/>
       <c r="AD485" s="13"/>
@@ -26605,7 +26615,7 @@
       <c r="X486" s="13"/>
       <c r="Y486" s="13"/>
       <c r="Z486" s="13"/>
-      <c r="AA486" s="13"/>
+      <c r="AA486" s="34"/>
       <c r="AB486" s="13"/>
       <c r="AC486" s="13"/>
       <c r="AD486" s="13"/>
@@ -26639,7 +26649,7 @@
       <c r="X487" s="13"/>
       <c r="Y487" s="13"/>
       <c r="Z487" s="13"/>
-      <c r="AA487" s="13"/>
+      <c r="AA487" s="34"/>
       <c r="AB487" s="13"/>
       <c r="AC487" s="13"/>
       <c r="AD487" s="13"/>
@@ -26673,7 +26683,7 @@
       <c r="X488" s="13"/>
       <c r="Y488" s="13"/>
       <c r="Z488" s="13"/>
-      <c r="AA488" s="13"/>
+      <c r="AA488" s="34"/>
       <c r="AB488" s="13"/>
       <c r="AC488" s="13"/>
       <c r="AD488" s="13"/>
@@ -26707,7 +26717,7 @@
       <c r="X489" s="13"/>
       <c r="Y489" s="13"/>
       <c r="Z489" s="13"/>
-      <c r="AA489" s="13"/>
+      <c r="AA489" s="34"/>
       <c r="AB489" s="13"/>
       <c r="AC489" s="13"/>
       <c r="AD489" s="13"/>
@@ -26741,7 +26751,7 @@
       <c r="X490" s="13"/>
       <c r="Y490" s="13"/>
       <c r="Z490" s="13"/>
-      <c r="AA490" s="13"/>
+      <c r="AA490" s="34"/>
       <c r="AB490" s="13"/>
       <c r="AC490" s="13"/>
       <c r="AD490" s="13"/>
@@ -26775,7 +26785,7 @@
       <c r="X491" s="13"/>
       <c r="Y491" s="13"/>
       <c r="Z491" s="13"/>
-      <c r="AA491" s="13"/>
+      <c r="AA491" s="34"/>
       <c r="AB491" s="13"/>
       <c r="AC491" s="13"/>
       <c r="AD491" s="13"/>
@@ -26809,7 +26819,7 @@
       <c r="X492" s="13"/>
       <c r="Y492" s="13"/>
       <c r="Z492" s="13"/>
-      <c r="AA492" s="13"/>
+      <c r="AA492" s="34"/>
       <c r="AB492" s="13"/>
       <c r="AC492" s="13"/>
       <c r="AD492" s="13"/>
@@ -26843,7 +26853,7 @@
       <c r="X493" s="13"/>
       <c r="Y493" s="13"/>
       <c r="Z493" s="13"/>
-      <c r="AA493" s="13"/>
+      <c r="AA493" s="34"/>
       <c r="AB493" s="13"/>
       <c r="AC493" s="13"/>
       <c r="AD493" s="13"/>
@@ -26877,7 +26887,7 @@
       <c r="X494" s="13"/>
       <c r="Y494" s="13"/>
       <c r="Z494" s="13"/>
-      <c r="AA494" s="13"/>
+      <c r="AA494" s="34"/>
       <c r="AB494" s="13"/>
       <c r="AC494" s="13"/>
       <c r="AD494" s="13"/>
@@ -26911,7 +26921,7 @@
       <c r="X495" s="13"/>
       <c r="Y495" s="13"/>
       <c r="Z495" s="13"/>
-      <c r="AA495" s="13"/>
+      <c r="AA495" s="34"/>
       <c r="AB495" s="13"/>
       <c r="AC495" s="13"/>
       <c r="AD495" s="13"/>
@@ -26945,7 +26955,7 @@
       <c r="X496" s="13"/>
       <c r="Y496" s="13"/>
       <c r="Z496" s="13"/>
-      <c r="AA496" s="13"/>
+      <c r="AA496" s="34"/>
       <c r="AB496" s="13"/>
       <c r="AC496" s="13"/>
       <c r="AD496" s="13"/>
@@ -26979,7 +26989,7 @@
       <c r="X497" s="13"/>
       <c r="Y497" s="13"/>
       <c r="Z497" s="13"/>
-      <c r="AA497" s="13"/>
+      <c r="AA497" s="34"/>
       <c r="AB497" s="13"/>
       <c r="AC497" s="13"/>
       <c r="AD497" s="13"/>
@@ -27013,7 +27023,7 @@
       <c r="X498" s="13"/>
       <c r="Y498" s="13"/>
       <c r="Z498" s="13"/>
-      <c r="AA498" s="13"/>
+      <c r="AA498" s="34"/>
       <c r="AB498" s="13"/>
       <c r="AC498" s="13"/>
       <c r="AD498" s="13"/>
@@ -27047,7 +27057,7 @@
       <c r="X499" s="13"/>
       <c r="Y499" s="13"/>
       <c r="Z499" s="13"/>
-      <c r="AA499" s="13"/>
+      <c r="AA499" s="34"/>
       <c r="AB499" s="13"/>
       <c r="AC499" s="13"/>
       <c r="AD499" s="13"/>
@@ -27081,7 +27091,7 @@
       <c r="X500" s="13"/>
       <c r="Y500" s="13"/>
       <c r="Z500" s="13"/>
-      <c r="AA500" s="13"/>
+      <c r="AA500" s="34"/>
       <c r="AB500" s="13"/>
       <c r="AC500" s="13"/>
       <c r="AD500" s="13"/>
@@ -27118,7 +27128,7 @@
       <formula>OR($L8="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -27131,6 +27141,7 @@
       <formula1>INDIRECT(SUBSTITUTE($AB8," ","_"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="AA8:AA500" xr:uid="{B204CDA7-FB33-DB4E-91DC-3DEE95D43266}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -27227,7 +27238,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>Z8:AA500</xm:sqref>
+          <xm:sqref>Z8:Z500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{368B6C73-4639-1545-829F-99B9B86A8384}">
           <x14:formula1>
@@ -27245,7 +27256,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294DF251-0142-7F42-AE19-CE025BFF4EB4}">
   <dimension ref="A1:J500"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -27254,8 +27267,8 @@
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29.5" customWidth="1"/>
     <col min="8" max="9" width="27.6640625" customWidth="1"/>
     <col min="10" max="10" width="24.33203125" customWidth="1"/>
   </cols>
@@ -32880,9 +32893,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{78D45380-7B14-D545-BE47-7320A88646CD}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{45363A0D-79CE-3647-BF12-A5096C413C0F}">
           <x14:formula1>
-            <xm:f>Index!#REF!</xm:f>
+            <xm:f>Index!$C$2:$C$11</xm:f>
           </x14:formula1>
           <xm:sqref>B4:B500</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
Added test to verify if a dict was None before accessing an item. Modified Library Size cell format in sample submission to remove decimal spaces.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_submission_v3_13_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_submission_v3_13_0.xlsx
@@ -332,6 +332,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Used for index validation. If left empty, the validation will be skipped.</t>
         </r>
@@ -9295,6 +9296,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -9516,7 +9518,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -9746,9 +9748,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1559880</xdr:colOff>
+      <xdr:colOff>1559520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>47160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9763,7 +9765,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="76320" y="28440"/>
-          <a:ext cx="1483560" cy="542880"/>
+          <a:ext cx="1483200" cy="542520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -26867,7 +26869,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.17"/>

</xml_diff>